<commit_message>
Add bus data for 15 southbound and 14
</commit_message>
<xml_diff>
--- a/data/bus_data.xlsx
+++ b/data/bus_data.xlsx
@@ -8,14 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/efc7ce48255d0cb5/Documents/2023 S2/COSC345/COSC345-Game/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92D09202-F985-4960-AFF2-A8F234A16CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="166" documentId="8_{92D09202-F985-4960-AFF2-A8F234A16CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80325E16-2F38-482A-A44E-F790A87982D1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{08F58157-5B37-470B-8714-523729044959}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="9" xr2:uid="{08F58157-5B37-470B-8714-523729044959}"/>
   </bookViews>
   <sheets>
-    <sheet name="15 M-F" sheetId="1" r:id="rId1"/>
-    <sheet name="15 Sat" sheetId="2" r:id="rId2"/>
-    <sheet name="15 Sun" sheetId="3" r:id="rId3"/>
+    <sheet name="15N M-F" sheetId="1" r:id="rId1"/>
+    <sheet name="15N Sat" sheetId="2" r:id="rId2"/>
+    <sheet name="15N Sun" sheetId="3" r:id="rId3"/>
+    <sheet name="15S M-F" sheetId="5" r:id="rId4"/>
+    <sheet name="15S Sat" sheetId="6" r:id="rId5"/>
+    <sheet name="15S Sun" sheetId="7" r:id="rId6"/>
+    <sheet name="14PC M-F" sheetId="8" r:id="rId7"/>
+    <sheet name="14PC Sat" sheetId="9" r:id="rId8"/>
+    <sheet name="14C M-F" sheetId="10" r:id="rId9"/>
+    <sheet name="14C Sat" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="671">
   <si>
     <t>5:50am</t>
   </si>
@@ -1031,6 +1038,1026 @@
   </si>
   <si>
     <t>Forth St, Leith Bridge</t>
+  </si>
+  <si>
+    <t>216 Highgate</t>
+  </si>
+  <si>
+    <t>Mornington, Mailer St</t>
+  </si>
+  <si>
+    <t>168 Hillside Rd</t>
+  </si>
+  <si>
+    <t>6:00am</t>
+  </si>
+  <si>
+    <t>6:30am</t>
+  </si>
+  <si>
+    <t>7:00am</t>
+  </si>
+  <si>
+    <t>7:30am</t>
+  </si>
+  <si>
+    <t>8:00am</t>
+  </si>
+  <si>
+    <t>8:30am</t>
+  </si>
+  <si>
+    <t>9:30am</t>
+  </si>
+  <si>
+    <t>10:30am</t>
+  </si>
+  <si>
+    <t>11:30am</t>
+  </si>
+  <si>
+    <t>12:30pm</t>
+  </si>
+  <si>
+    <t>6:16am</t>
+  </si>
+  <si>
+    <t>6:46am</t>
+  </si>
+  <si>
+    <t>7:16am</t>
+  </si>
+  <si>
+    <t>7:46am</t>
+  </si>
+  <si>
+    <t>8:16am</t>
+  </si>
+  <si>
+    <t>8:46am</t>
+  </si>
+  <si>
+    <t>9:16am</t>
+  </si>
+  <si>
+    <t>9:46am</t>
+  </si>
+  <si>
+    <t>10:16am</t>
+  </si>
+  <si>
+    <t>10:46am</t>
+  </si>
+  <si>
+    <t>11:16am</t>
+  </si>
+  <si>
+    <t>11:46am</t>
+  </si>
+  <si>
+    <t>12:16pm</t>
+  </si>
+  <si>
+    <t>12:46pm</t>
+  </si>
+  <si>
+    <t>1:16pm</t>
+  </si>
+  <si>
+    <t>7:52am</t>
+  </si>
+  <si>
+    <t>8:22am</t>
+  </si>
+  <si>
+    <t>6:28am</t>
+  </si>
+  <si>
+    <t>6:58am</t>
+  </si>
+  <si>
+    <t>7:28am</t>
+  </si>
+  <si>
+    <t>8:01am</t>
+  </si>
+  <si>
+    <t>8:31am</t>
+  </si>
+  <si>
+    <t>8:58am</t>
+  </si>
+  <si>
+    <t>9:58am</t>
+  </si>
+  <si>
+    <t>10:58am</t>
+  </si>
+  <si>
+    <t>11:58am</t>
+  </si>
+  <si>
+    <t>12:58pm</t>
+  </si>
+  <si>
+    <t>6:33am</t>
+  </si>
+  <si>
+    <t>7:03am</t>
+  </si>
+  <si>
+    <t>7:33am</t>
+  </si>
+  <si>
+    <t>8:05am</t>
+  </si>
+  <si>
+    <t>8:35am</t>
+  </si>
+  <si>
+    <t>9:33am</t>
+  </si>
+  <si>
+    <t>10:33am</t>
+  </si>
+  <si>
+    <t>11:33am</t>
+  </si>
+  <si>
+    <t>12:33pm</t>
+  </si>
+  <si>
+    <t>1:33pm</t>
+  </si>
+  <si>
+    <t>1:30pm</t>
+  </si>
+  <si>
+    <t>2:30pm</t>
+  </si>
+  <si>
+    <t>3:30pm</t>
+  </si>
+  <si>
+    <t>4:30pm</t>
+  </si>
+  <si>
+    <t>5:30pm</t>
+  </si>
+  <si>
+    <t>6:30pm</t>
+  </si>
+  <si>
+    <t>1:46pm</t>
+  </si>
+  <si>
+    <t>2:16pm</t>
+  </si>
+  <si>
+    <t>2:46pm</t>
+  </si>
+  <si>
+    <t>3:16pm</t>
+  </si>
+  <si>
+    <t>3:46pm</t>
+  </si>
+  <si>
+    <t>4:16pm</t>
+  </si>
+  <si>
+    <t>4:46pm</t>
+  </si>
+  <si>
+    <t>5:16pm</t>
+  </si>
+  <si>
+    <t>5:46pm</t>
+  </si>
+  <si>
+    <t>6:16pm</t>
+  </si>
+  <si>
+    <t>6:46pm</t>
+  </si>
+  <si>
+    <t>7:46pm</t>
+  </si>
+  <si>
+    <t>8:46pm</t>
+  </si>
+  <si>
+    <t>9:46pm</t>
+  </si>
+  <si>
+    <t>10:46pm</t>
+  </si>
+  <si>
+    <t>5:22pm</t>
+  </si>
+  <si>
+    <t>5:52pm</t>
+  </si>
+  <si>
+    <t>7:51pm</t>
+  </si>
+  <si>
+    <t>8:51pm</t>
+  </si>
+  <si>
+    <t>9:51pm</t>
+  </si>
+  <si>
+    <t>10:51pm</t>
+  </si>
+  <si>
+    <t>1:58pm</t>
+  </si>
+  <si>
+    <t>2:58pm</t>
+  </si>
+  <si>
+    <t>3:58pm</t>
+  </si>
+  <si>
+    <t>4:58pm</t>
+  </si>
+  <si>
+    <t>5:31pm</t>
+  </si>
+  <si>
+    <t>6:01pm</t>
+  </si>
+  <si>
+    <t>6:58pm</t>
+  </si>
+  <si>
+    <t>2:33pm</t>
+  </si>
+  <si>
+    <t>3:33pm</t>
+  </si>
+  <si>
+    <t>4:33pm</t>
+  </si>
+  <si>
+    <t>6:05pm</t>
+  </si>
+  <si>
+    <t>6:33pm</t>
+  </si>
+  <si>
+    <t>8:03pm</t>
+  </si>
+  <si>
+    <t>9:03pm</t>
+  </si>
+  <si>
+    <t>10:03pm</t>
+  </si>
+  <si>
+    <t>11:03pm</t>
+  </si>
+  <si>
+    <t>9:31am</t>
+  </si>
+  <si>
+    <t>10:31am</t>
+  </si>
+  <si>
+    <t>11:31am</t>
+  </si>
+  <si>
+    <t>12:31pm</t>
+  </si>
+  <si>
+    <t>1:31pm</t>
+  </si>
+  <si>
+    <t>2:31pm</t>
+  </si>
+  <si>
+    <t>3:31pm</t>
+  </si>
+  <si>
+    <t>4:31pm</t>
+  </si>
+  <si>
+    <t>6:31pm</t>
+  </si>
+  <si>
+    <t>7:31pm</t>
+  </si>
+  <si>
+    <t>8:31pm</t>
+  </si>
+  <si>
+    <t>9:31pm</t>
+  </si>
+  <si>
+    <t>10:31pm</t>
+  </si>
+  <si>
+    <t>11:31pm</t>
+  </si>
+  <si>
+    <t>8:37am</t>
+  </si>
+  <si>
+    <t>9:37am</t>
+  </si>
+  <si>
+    <t>10:37am</t>
+  </si>
+  <si>
+    <t>11:37am</t>
+  </si>
+  <si>
+    <t>12:37pm</t>
+  </si>
+  <si>
+    <t>1:37pm</t>
+  </si>
+  <si>
+    <t>2:37pm</t>
+  </si>
+  <si>
+    <t>3:37pm</t>
+  </si>
+  <si>
+    <t>4:37pm</t>
+  </si>
+  <si>
+    <t>5:37pm</t>
+  </si>
+  <si>
+    <t>6:37pm</t>
+  </si>
+  <si>
+    <t>7:37pm</t>
+  </si>
+  <si>
+    <t>8:37pm</t>
+  </si>
+  <si>
+    <t>9:37pm</t>
+  </si>
+  <si>
+    <t>10:37pm</t>
+  </si>
+  <si>
+    <t>11:37pm</t>
+  </si>
+  <si>
+    <t>11:46pm</t>
+  </si>
+  <si>
+    <t>7:16pm</t>
+  </si>
+  <si>
+    <t>9:22am</t>
+  </si>
+  <si>
+    <t>10:22am</t>
+  </si>
+  <si>
+    <t>11:22am</t>
+  </si>
+  <si>
+    <t>12:22pm</t>
+  </si>
+  <si>
+    <t>1:22pm</t>
+  </si>
+  <si>
+    <t>2:22pm</t>
+  </si>
+  <si>
+    <t>3:22pm</t>
+  </si>
+  <si>
+    <t>4:22pm</t>
+  </si>
+  <si>
+    <t>6:22pm</t>
+  </si>
+  <si>
+    <t>7:22pm</t>
+  </si>
+  <si>
+    <t>Harrington St, cnr Fox St</t>
+  </si>
+  <si>
+    <t>SH88, St Leonards Dr Nth</t>
+  </si>
+  <si>
+    <t>Bus Hub Stop G</t>
+  </si>
+  <si>
+    <t>6:10a.m.</t>
+  </si>
+  <si>
+    <t>6:40a.m.</t>
+  </si>
+  <si>
+    <t>7:10a.m.</t>
+  </si>
+  <si>
+    <t>7:30a.m.</t>
+  </si>
+  <si>
+    <t>7:50a.m.</t>
+  </si>
+  <si>
+    <t>8:10a.m.</t>
+  </si>
+  <si>
+    <t>8:40a.m.</t>
+  </si>
+  <si>
+    <t>9:10a.m.</t>
+  </si>
+  <si>
+    <t>9:40a.m.</t>
+  </si>
+  <si>
+    <t>10:10a.m.</t>
+  </si>
+  <si>
+    <t>10:40a.m.</t>
+  </si>
+  <si>
+    <t>11:10a.m.</t>
+  </si>
+  <si>
+    <t>11:40a.m.</t>
+  </si>
+  <si>
+    <t>12:10p.m.</t>
+  </si>
+  <si>
+    <t>12:40p.m.</t>
+  </si>
+  <si>
+    <t>1:10p.m.</t>
+  </si>
+  <si>
+    <t>6:23a.m.</t>
+  </si>
+  <si>
+    <t>6:53a.m.</t>
+  </si>
+  <si>
+    <t>7:23a.m.</t>
+  </si>
+  <si>
+    <t>7:43a.m.</t>
+  </si>
+  <si>
+    <t>8:03a.m.</t>
+  </si>
+  <si>
+    <t>8:23a.m.</t>
+  </si>
+  <si>
+    <t>8:53a.m.</t>
+  </si>
+  <si>
+    <t>9:23a.m.</t>
+  </si>
+  <si>
+    <t>9:53a.m.</t>
+  </si>
+  <si>
+    <t>10:23a.m.</t>
+  </si>
+  <si>
+    <t>10:53a.m.</t>
+  </si>
+  <si>
+    <t>11:23a.m.</t>
+  </si>
+  <si>
+    <t>11:53a.m.</t>
+  </si>
+  <si>
+    <t>12:23p.m.</t>
+  </si>
+  <si>
+    <t>12:53p.m.</t>
+  </si>
+  <si>
+    <t>1:23p.m.</t>
+  </si>
+  <si>
+    <t>6:41a.m.</t>
+  </si>
+  <si>
+    <t>7:11a.m.</t>
+  </si>
+  <si>
+    <t>7:41a.m.</t>
+  </si>
+  <si>
+    <t>8:01a.m.</t>
+  </si>
+  <si>
+    <t>8:21a.m.</t>
+  </si>
+  <si>
+    <t>8:41a.m.</t>
+  </si>
+  <si>
+    <t>9:11a.m.</t>
+  </si>
+  <si>
+    <t>9:41a.m.</t>
+  </si>
+  <si>
+    <t>10:11a.m.</t>
+  </si>
+  <si>
+    <t>10:41a.m.</t>
+  </si>
+  <si>
+    <t>11:11a.m.</t>
+  </si>
+  <si>
+    <t>11:41a.m.</t>
+  </si>
+  <si>
+    <t>12:11p.m.</t>
+  </si>
+  <si>
+    <t>12:41p.m.</t>
+  </si>
+  <si>
+    <t>1:11p.m.</t>
+  </si>
+  <si>
+    <t>1:41p.m.</t>
+  </si>
+  <si>
+    <t>1:40p.m.</t>
+  </si>
+  <si>
+    <t>2:10p.m.</t>
+  </si>
+  <si>
+    <t>2:40p.m.</t>
+  </si>
+  <si>
+    <t>3:10p.m.</t>
+  </si>
+  <si>
+    <t>3:40p.m.</t>
+  </si>
+  <si>
+    <t>4:10p.m.</t>
+  </si>
+  <si>
+    <t>4:40p.m.</t>
+  </si>
+  <si>
+    <t>5:10p.m.</t>
+  </si>
+  <si>
+    <t>5:40p.m.</t>
+  </si>
+  <si>
+    <t>6:10p.m.</t>
+  </si>
+  <si>
+    <t>6:40p.m.</t>
+  </si>
+  <si>
+    <t>7:10p.m.</t>
+  </si>
+  <si>
+    <t>8:10p.m.</t>
+  </si>
+  <si>
+    <t>9:10p.m.</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>10:10p.m.</t>
+  </si>
+  <si>
+    <t>11:10p.m.</t>
+  </si>
+  <si>
+    <t>1:53p.m.</t>
+  </si>
+  <si>
+    <t>2:23p.m.</t>
+  </si>
+  <si>
+    <t>2:53p.m.</t>
+  </si>
+  <si>
+    <t>3:23p.m.</t>
+  </si>
+  <si>
+    <t>3:53p.m.</t>
+  </si>
+  <si>
+    <t>4:23p.m.</t>
+  </si>
+  <si>
+    <t>4:53p.m.</t>
+  </si>
+  <si>
+    <t>5:23p.m.</t>
+  </si>
+  <si>
+    <t>5:53p.m.</t>
+  </si>
+  <si>
+    <t>6:23p.m.</t>
+  </si>
+  <si>
+    <t>6:53p.m.</t>
+  </si>
+  <si>
+    <t>7:23p.m.</t>
+  </si>
+  <si>
+    <t>8:23p.m.</t>
+  </si>
+  <si>
+    <t>9:23p.m.</t>
+  </si>
+  <si>
+    <t>10:23p.m.</t>
+  </si>
+  <si>
+    <t>11:23p.m.</t>
+  </si>
+  <si>
+    <t>2:11p.m.</t>
+  </si>
+  <si>
+    <t>2:41p.m.</t>
+  </si>
+  <si>
+    <t>3:11p.m.</t>
+  </si>
+  <si>
+    <t>3:41p.m.</t>
+  </si>
+  <si>
+    <t>4:11p.m.</t>
+  </si>
+  <si>
+    <t>4:41p.m.</t>
+  </si>
+  <si>
+    <t>5:11p.m.</t>
+  </si>
+  <si>
+    <t>5:41p.m.</t>
+  </si>
+  <si>
+    <t>6:11p.m.</t>
+  </si>
+  <si>
+    <t>6:41p.m.</t>
+  </si>
+  <si>
+    <t>7:11p.m.</t>
+  </si>
+  <si>
+    <t>7:41p.m.</t>
+  </si>
+  <si>
+    <t>8:41p.m.</t>
+  </si>
+  <si>
+    <t>9:41p.m.</t>
+  </si>
+  <si>
+    <t>10:41p.m.</t>
+  </si>
+  <si>
+    <t>11:41p.m.</t>
+  </si>
+  <si>
+    <t>Bus Route</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Northbound</t>
+  </si>
+  <si>
+    <t>Monday-Friday</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Southbound</t>
+  </si>
+  <si>
+    <t>Port Chalmers -&gt; City</t>
+  </si>
+  <si>
+    <t>F: Friday only</t>
+  </si>
+  <si>
+    <t>Some of these don't run on public holidays but these were ignored</t>
+  </si>
+  <si>
+    <t>Bus Hub Stop B</t>
+  </si>
+  <si>
+    <t>Careys Bay Hotel</t>
+  </si>
+  <si>
+    <t>6:31a.m.</t>
+  </si>
+  <si>
+    <t>7:01a.m.</t>
+  </si>
+  <si>
+    <t>7:31a.m.</t>
+  </si>
+  <si>
+    <t>8:31a.m.</t>
+  </si>
+  <si>
+    <t>9:01a.m.</t>
+  </si>
+  <si>
+    <t>9:31a.m. 10:01a.m. 10:31a.m. 11:01a.m. 11:31a.m. 12:01p.m. 12:31p.m.</t>
+  </si>
+  <si>
+    <t>1:01p.m.</t>
+  </si>
+  <si>
+    <t>1:31p.m.</t>
+  </si>
+  <si>
+    <t>2:01p.m.</t>
+  </si>
+  <si>
+    <t>6:47a.m.</t>
+  </si>
+  <si>
+    <t>7:17a.m.</t>
+  </si>
+  <si>
+    <t>7:47a.m.</t>
+  </si>
+  <si>
+    <t>8:17a.m.</t>
+  </si>
+  <si>
+    <t>8:47a.m.</t>
+  </si>
+  <si>
+    <t>9:17a.m.</t>
+  </si>
+  <si>
+    <t>9:47a.m. 10:17a.m. 10:47a.m. 11:17a.m. 11:47a.m. 12:17p.m. 12:47p.m.</t>
+  </si>
+  <si>
+    <t>1:17p.m.</t>
+  </si>
+  <si>
+    <t>1:47p.m.</t>
+  </si>
+  <si>
+    <t>2:17p.m.</t>
+  </si>
+  <si>
+    <t>9:31a.m.</t>
+  </si>
+  <si>
+    <t>10:01a.m. 10:31a.m. 11:01a.m. 11:31a.m. 12:01p.m. 12:31p.m. 1:01p.m.</t>
+  </si>
+  <si>
+    <t>2:31p.m.</t>
+  </si>
+  <si>
+    <t>7:05a.m.</t>
+  </si>
+  <si>
+    <t>7:35a.m.</t>
+  </si>
+  <si>
+    <t>8:05a.m.</t>
+  </si>
+  <si>
+    <t>8:35a.m.</t>
+  </si>
+  <si>
+    <t>9:05a.m.</t>
+  </si>
+  <si>
+    <t>9:35a.m.</t>
+  </si>
+  <si>
+    <t>10:05a.m. 10:35a.m. 11:05a.m. 11:35a.m. 12:05p.m. 12:35p.m. 1:05p.m.</t>
+  </si>
+  <si>
+    <t>1:35p.m.</t>
+  </si>
+  <si>
+    <t>2:05p.m.</t>
+  </si>
+  <si>
+    <t>2:35p.m.</t>
+  </si>
+  <si>
+    <t>2:31p.m. 3:01p.m. 3:31p.m. 4:01p.m. 4:31p.m. 5:01p.m. 5:31p.m. 6:01p.m. 6:31p.m. 7:01p.m. 7:31p.m. 8:31p.m. 9:31p.m. F 10:31p.m. F 11:31p.m</t>
+  </si>
+  <si>
+    <t>2:47p.m. 3:17p.m. 3:47p.m. 4:17p.m. 4:47p.m. 5:17p.m. 5:47p.m. 6:17p.m. 6:47p.m. 7:17p.m. 7:47p.m. 8:47p.m. 9:47p.m. F 10:47p.m. F 11:47p.m.</t>
+  </si>
+  <si>
+    <t>3:01p.m. 3:31p.m. 4:01p.m. 4:31p.m. 5:01p.m. 5:31p.m. 6:01p.m. 6:31p.m. 7:01p.m. 7:31p.m. 8:01p.m. 9:01p.m. 10:01p.m. F 11:01p.m. F 12:01a.m.</t>
+  </si>
+  <si>
+    <t>3:05p.m. 3:35p.m. 4:05p.m. 4:35p.m. 5:05p.m. 5:35p.m. 6:05p.m. 6:35p.m. 7:05p.m. 7:35p.m. 8:05p.m. 9:05p.m. 10:05p.m. F 11:05p.m. F 12:05a.m.</t>
+  </si>
+  <si>
+    <t>City -&gt; Port Chalmers</t>
+  </si>
+  <si>
+    <t>10:31a.m.</t>
+  </si>
+  <si>
+    <t>11:31a.m.</t>
+  </si>
+  <si>
+    <t>12:31p.m.</t>
+  </si>
+  <si>
+    <t>3:31p.m.</t>
+  </si>
+  <si>
+    <t>4:31p.m.</t>
+  </si>
+  <si>
+    <t>5:31p.m.</t>
+  </si>
+  <si>
+    <t>6:31p.m.</t>
+  </si>
+  <si>
+    <t>7:31p.m.</t>
+  </si>
+  <si>
+    <t>8:31p.m.</t>
+  </si>
+  <si>
+    <t>9:31p.m.</t>
+  </si>
+  <si>
+    <t>10:31p.m.</t>
+  </si>
+  <si>
+    <t>11:31p.m.</t>
+  </si>
+  <si>
+    <t>9:47a.m.</t>
+  </si>
+  <si>
+    <t>10:47a.m.</t>
+  </si>
+  <si>
+    <t>11:47a.m.</t>
+  </si>
+  <si>
+    <t>12:47p.m.</t>
+  </si>
+  <si>
+    <t>2:47p.m.</t>
+  </si>
+  <si>
+    <t>3:47p.m.</t>
+  </si>
+  <si>
+    <t>4:47p.m.</t>
+  </si>
+  <si>
+    <t>5:47p.m.</t>
+  </si>
+  <si>
+    <t>6:47p.m.</t>
+  </si>
+  <si>
+    <t>7:47p.m.</t>
+  </si>
+  <si>
+    <t>8:47p.m.</t>
+  </si>
+  <si>
+    <t>9:47p.m.</t>
+  </si>
+  <si>
+    <t>10:47p.m.</t>
+  </si>
+  <si>
+    <t>11:47p.m.</t>
+  </si>
+  <si>
+    <t>10:01a.m.</t>
+  </si>
+  <si>
+    <t>11:01a.m.</t>
+  </si>
+  <si>
+    <t>12:01p.m.</t>
+  </si>
+  <si>
+    <t>3:01p.m.</t>
+  </si>
+  <si>
+    <t>4:01p.m.</t>
+  </si>
+  <si>
+    <t>5:01p.m.</t>
+  </si>
+  <si>
+    <t>6:01p.m.</t>
+  </si>
+  <si>
+    <t>7:01p.m.</t>
+  </si>
+  <si>
+    <t>8:01p.m.</t>
+  </si>
+  <si>
+    <t>9:01p.m.</t>
+  </si>
+  <si>
+    <t>10:01p.m.</t>
+  </si>
+  <si>
+    <t>11:01p.m.</t>
+  </si>
+  <si>
+    <t>12:01a.m.</t>
+  </si>
+  <si>
+    <t>10:05a.m.</t>
+  </si>
+  <si>
+    <t>11:05a.m.</t>
+  </si>
+  <si>
+    <t>12:05p.m.</t>
+  </si>
+  <si>
+    <t>1:05p.m.</t>
+  </si>
+  <si>
+    <t>3:05p.m.</t>
+  </si>
+  <si>
+    <t>4:05p.m.</t>
+  </si>
+  <si>
+    <t>5:05p.m.</t>
+  </si>
+  <si>
+    <t>6:05p.m.</t>
+  </si>
+  <si>
+    <t>7:05p.m.</t>
+  </si>
+  <si>
+    <t>8:05p.m.</t>
+  </si>
+  <si>
+    <t>9:05p.m.</t>
+  </si>
+  <si>
+    <t>10:05p.m.</t>
+  </si>
+  <si>
+    <t>11:05p.m.</t>
+  </si>
+  <si>
+    <t>12:05a.m.</t>
   </si>
 </sst>
 </file>
@@ -1382,10 +2409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D2E1A5-2446-445B-A24B-7B29F9CDA543}">
-  <dimension ref="A1:AF6"/>
+  <dimension ref="A1:AF9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:AF6"/>
+      <selection activeCell="B8" sqref="B8:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1981,6 +3008,292 @@
         <v>179</v>
       </c>
     </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>566</v>
+      </c>
+      <c r="C8" t="s">
+        <v>567</v>
+      </c>
+      <c r="D8" t="s">
+        <v>568</v>
+      </c>
+      <c r="E8" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>575</v>
+      </c>
+      <c r="D9" t="s">
+        <v>571</v>
+      </c>
+      <c r="E9" t="s">
+        <v>572</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27BA5E9F-3C21-4944-A859-C18E0E66A19E}">
+  <dimension ref="A1:Q7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B1" t="s">
+        <v>584</v>
+      </c>
+      <c r="C1" t="s">
+        <v>600</v>
+      </c>
+      <c r="D1" t="s">
+        <v>618</v>
+      </c>
+      <c r="E1" t="s">
+        <v>619</v>
+      </c>
+      <c r="F1" t="s">
+        <v>620</v>
+      </c>
+      <c r="G1" t="s">
+        <v>588</v>
+      </c>
+      <c r="H1" t="s">
+        <v>602</v>
+      </c>
+      <c r="I1" t="s">
+        <v>621</v>
+      </c>
+      <c r="J1" t="s">
+        <v>622</v>
+      </c>
+      <c r="K1" t="s">
+        <v>623</v>
+      </c>
+      <c r="L1" t="s">
+        <v>624</v>
+      </c>
+      <c r="M1" t="s">
+        <v>625</v>
+      </c>
+      <c r="N1" t="s">
+        <v>626</v>
+      </c>
+      <c r="O1" t="s">
+        <v>627</v>
+      </c>
+      <c r="P1" t="s">
+        <v>628</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B2" t="s">
+        <v>594</v>
+      </c>
+      <c r="C2" t="s">
+        <v>630</v>
+      </c>
+      <c r="D2" t="s">
+        <v>631</v>
+      </c>
+      <c r="E2" t="s">
+        <v>632</v>
+      </c>
+      <c r="F2" t="s">
+        <v>633</v>
+      </c>
+      <c r="G2" t="s">
+        <v>598</v>
+      </c>
+      <c r="H2" t="s">
+        <v>634</v>
+      </c>
+      <c r="I2" t="s">
+        <v>635</v>
+      </c>
+      <c r="J2" t="s">
+        <v>636</v>
+      </c>
+      <c r="K2" t="s">
+        <v>637</v>
+      </c>
+      <c r="L2" t="s">
+        <v>638</v>
+      </c>
+      <c r="M2" t="s">
+        <v>639</v>
+      </c>
+      <c r="N2" t="s">
+        <v>640</v>
+      </c>
+      <c r="O2" t="s">
+        <v>641</v>
+      </c>
+      <c r="P2" t="s">
+        <v>642</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>580</v>
+      </c>
+      <c r="B3" t="s">
+        <v>585</v>
+      </c>
+      <c r="C3" t="s">
+        <v>644</v>
+      </c>
+      <c r="D3" t="s">
+        <v>645</v>
+      </c>
+      <c r="E3" t="s">
+        <v>646</v>
+      </c>
+      <c r="F3" t="s">
+        <v>587</v>
+      </c>
+      <c r="G3" t="s">
+        <v>589</v>
+      </c>
+      <c r="H3" t="s">
+        <v>647</v>
+      </c>
+      <c r="I3" t="s">
+        <v>648</v>
+      </c>
+      <c r="J3" t="s">
+        <v>649</v>
+      </c>
+      <c r="K3" t="s">
+        <v>650</v>
+      </c>
+      <c r="L3" t="s">
+        <v>651</v>
+      </c>
+      <c r="M3" t="s">
+        <v>652</v>
+      </c>
+      <c r="N3" t="s">
+        <v>653</v>
+      </c>
+      <c r="O3" t="s">
+        <v>654</v>
+      </c>
+      <c r="P3" t="s">
+        <v>655</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>466</v>
+      </c>
+      <c r="B4" t="s">
+        <v>607</v>
+      </c>
+      <c r="C4" t="s">
+        <v>657</v>
+      </c>
+      <c r="D4" t="s">
+        <v>658</v>
+      </c>
+      <c r="E4" t="s">
+        <v>659</v>
+      </c>
+      <c r="F4" t="s">
+        <v>660</v>
+      </c>
+      <c r="G4" t="s">
+        <v>611</v>
+      </c>
+      <c r="H4" t="s">
+        <v>661</v>
+      </c>
+      <c r="I4" t="s">
+        <v>662</v>
+      </c>
+      <c r="J4" t="s">
+        <v>663</v>
+      </c>
+      <c r="K4" t="s">
+        <v>664</v>
+      </c>
+      <c r="L4" t="s">
+        <v>665</v>
+      </c>
+      <c r="M4" t="s">
+        <v>666</v>
+      </c>
+      <c r="N4" t="s">
+        <v>667</v>
+      </c>
+      <c r="O4" t="s">
+        <v>668</v>
+      </c>
+      <c r="P4" t="s">
+        <v>669</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>566</v>
+      </c>
+      <c r="C6" t="s">
+        <v>567</v>
+      </c>
+      <c r="D6" t="s">
+        <v>568</v>
+      </c>
+      <c r="E6" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>617</v>
+      </c>
+      <c r="D7" t="s">
+        <v>573</v>
+      </c>
+      <c r="E7" t="s">
+        <v>578</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1988,10 +3301,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FAA4CF-A924-4CCA-94BD-D8BB34C13E46}">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:Q6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2317,6 +3630,34 @@
         <v>324</v>
       </c>
     </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>566</v>
+      </c>
+      <c r="C8" t="s">
+        <v>567</v>
+      </c>
+      <c r="D8" t="s">
+        <v>568</v>
+      </c>
+      <c r="E8" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>570</v>
+      </c>
+      <c r="D9" t="s">
+        <v>573</v>
+      </c>
+      <c r="E9" t="s">
+        <v>572</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2324,10 +3665,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A38978-965C-41A3-80ED-94BB62F49761}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2563,6 +3904,1875 @@
         <v>312</v>
       </c>
     </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>566</v>
+      </c>
+      <c r="C8" t="s">
+        <v>567</v>
+      </c>
+      <c r="D8" t="s">
+        <v>568</v>
+      </c>
+      <c r="E8" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>570</v>
+      </c>
+      <c r="D9" t="s">
+        <v>574</v>
+      </c>
+      <c r="E9" t="s">
+        <v>572</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6111A1C1-8F73-4833-8C1A-4F04EC14CE6E}">
+  <dimension ref="A1:AE9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C1" t="s">
+        <v>335</v>
+      </c>
+      <c r="D1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E1" t="s">
+        <v>337</v>
+      </c>
+      <c r="F1" t="s">
+        <v>338</v>
+      </c>
+      <c r="G1" t="s">
+        <v>339</v>
+      </c>
+      <c r="H1" t="s">
+        <v>247</v>
+      </c>
+      <c r="I1" t="s">
+        <v>340</v>
+      </c>
+      <c r="J1" t="s">
+        <v>248</v>
+      </c>
+      <c r="K1" t="s">
+        <v>341</v>
+      </c>
+      <c r="L1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M1" t="s">
+        <v>342</v>
+      </c>
+      <c r="N1" t="s">
+        <v>250</v>
+      </c>
+      <c r="O1" t="s">
+        <v>343</v>
+      </c>
+      <c r="P1" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>381</v>
+      </c>
+      <c r="R1" t="s">
+        <v>252</v>
+      </c>
+      <c r="S1" t="s">
+        <v>382</v>
+      </c>
+      <c r="T1" t="s">
+        <v>253</v>
+      </c>
+      <c r="U1" t="s">
+        <v>383</v>
+      </c>
+      <c r="V1" t="s">
+        <v>254</v>
+      </c>
+      <c r="W1" t="s">
+        <v>384</v>
+      </c>
+      <c r="X1" t="s">
+        <v>255</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>385</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>256</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>386</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D2" t="s">
+        <v>346</v>
+      </c>
+      <c r="E2" t="s">
+        <v>347</v>
+      </c>
+      <c r="F2" t="s">
+        <v>348</v>
+      </c>
+      <c r="G2" t="s">
+        <v>349</v>
+      </c>
+      <c r="H2" t="s">
+        <v>350</v>
+      </c>
+      <c r="I2" t="s">
+        <v>351</v>
+      </c>
+      <c r="J2" t="s">
+        <v>352</v>
+      </c>
+      <c r="K2" t="s">
+        <v>353</v>
+      </c>
+      <c r="L2" t="s">
+        <v>354</v>
+      </c>
+      <c r="M2" t="s">
+        <v>355</v>
+      </c>
+      <c r="N2" t="s">
+        <v>356</v>
+      </c>
+      <c r="O2" t="s">
+        <v>357</v>
+      </c>
+      <c r="P2" t="s">
+        <v>358</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>387</v>
+      </c>
+      <c r="R2" t="s">
+        <v>388</v>
+      </c>
+      <c r="S2" t="s">
+        <v>389</v>
+      </c>
+      <c r="T2" t="s">
+        <v>390</v>
+      </c>
+      <c r="U2" t="s">
+        <v>391</v>
+      </c>
+      <c r="V2" t="s">
+        <v>392</v>
+      </c>
+      <c r="W2" t="s">
+        <v>393</v>
+      </c>
+      <c r="X2" t="s">
+        <v>394</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>395</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>396</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>397</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>398</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>399</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>400</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>359</v>
+      </c>
+      <c r="F3" t="s">
+        <v>360</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" t="s">
+        <v>44</v>
+      </c>
+      <c r="P3" t="s">
+        <v>315</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>120</v>
+      </c>
+      <c r="R3" t="s">
+        <v>121</v>
+      </c>
+      <c r="S3" t="s">
+        <v>122</v>
+      </c>
+      <c r="T3" t="s">
+        <v>123</v>
+      </c>
+      <c r="U3" t="s">
+        <v>124</v>
+      </c>
+      <c r="V3" t="s">
+        <v>125</v>
+      </c>
+      <c r="W3" t="s">
+        <v>126</v>
+      </c>
+      <c r="X3" t="s">
+        <v>402</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>403</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>129</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>404</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>405</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>406</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>333</v>
+      </c>
+      <c r="B4" t="s">
+        <v>361</v>
+      </c>
+      <c r="C4" t="s">
+        <v>362</v>
+      </c>
+      <c r="D4" t="s">
+        <v>363</v>
+      </c>
+      <c r="E4" t="s">
+        <v>364</v>
+      </c>
+      <c r="F4" t="s">
+        <v>365</v>
+      </c>
+      <c r="G4" t="s">
+        <v>366</v>
+      </c>
+      <c r="H4" t="s">
+        <v>291</v>
+      </c>
+      <c r="I4" t="s">
+        <v>367</v>
+      </c>
+      <c r="J4" t="s">
+        <v>292</v>
+      </c>
+      <c r="K4" t="s">
+        <v>368</v>
+      </c>
+      <c r="L4" t="s">
+        <v>293</v>
+      </c>
+      <c r="M4" t="s">
+        <v>369</v>
+      </c>
+      <c r="N4" t="s">
+        <v>294</v>
+      </c>
+      <c r="O4" t="s">
+        <v>370</v>
+      </c>
+      <c r="P4" t="s">
+        <v>295</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>408</v>
+      </c>
+      <c r="R4" t="s">
+        <v>296</v>
+      </c>
+      <c r="S4" t="s">
+        <v>409</v>
+      </c>
+      <c r="T4" t="s">
+        <v>297</v>
+      </c>
+      <c r="U4" t="s">
+        <v>410</v>
+      </c>
+      <c r="V4" t="s">
+        <v>298</v>
+      </c>
+      <c r="W4" t="s">
+        <v>411</v>
+      </c>
+      <c r="X4" t="s">
+        <v>412</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>413</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>300</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>414</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>161</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>162</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>163</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>325</v>
+      </c>
+      <c r="B5" t="s">
+        <v>371</v>
+      </c>
+      <c r="C5" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5" t="s">
+        <v>373</v>
+      </c>
+      <c r="E5" t="s">
+        <v>374</v>
+      </c>
+      <c r="F5" t="s">
+        <v>375</v>
+      </c>
+      <c r="G5" t="s">
+        <v>258</v>
+      </c>
+      <c r="H5" t="s">
+        <v>376</v>
+      </c>
+      <c r="I5" t="s">
+        <v>259</v>
+      </c>
+      <c r="J5" t="s">
+        <v>377</v>
+      </c>
+      <c r="K5" t="s">
+        <v>260</v>
+      </c>
+      <c r="L5" t="s">
+        <v>378</v>
+      </c>
+      <c r="M5" t="s">
+        <v>261</v>
+      </c>
+      <c r="N5" t="s">
+        <v>379</v>
+      </c>
+      <c r="O5" t="s">
+        <v>262</v>
+      </c>
+      <c r="P5" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>263</v>
+      </c>
+      <c r="R5" t="s">
+        <v>415</v>
+      </c>
+      <c r="S5" t="s">
+        <v>264</v>
+      </c>
+      <c r="T5" t="s">
+        <v>416</v>
+      </c>
+      <c r="U5" t="s">
+        <v>265</v>
+      </c>
+      <c r="V5" t="s">
+        <v>417</v>
+      </c>
+      <c r="W5" t="s">
+        <v>266</v>
+      </c>
+      <c r="X5" t="s">
+        <v>310</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>418</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>419</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>268</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>420</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>421</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>422</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>566</v>
+      </c>
+      <c r="C8" t="s">
+        <v>567</v>
+      </c>
+      <c r="D8" t="s">
+        <v>568</v>
+      </c>
+      <c r="E8" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>575</v>
+      </c>
+      <c r="D9" t="s">
+        <v>571</v>
+      </c>
+      <c r="E9" t="s">
+        <v>572</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B6">
+    <sortCondition descending="1" ref="B1:B6"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{486C7500-5AEE-4C77-AA7C-90D11E4B899C}">
+  <dimension ref="A1:Q8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J1" t="s">
+        <v>169</v>
+      </c>
+      <c r="K1" t="s">
+        <v>171</v>
+      </c>
+      <c r="L1" t="s">
+        <v>181</v>
+      </c>
+      <c r="M1" t="s">
+        <v>175</v>
+      </c>
+      <c r="N1" t="s">
+        <v>182</v>
+      </c>
+      <c r="O1" t="s">
+        <v>183</v>
+      </c>
+      <c r="P1" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C2" t="s">
+        <v>424</v>
+      </c>
+      <c r="D2" t="s">
+        <v>425</v>
+      </c>
+      <c r="E2" t="s">
+        <v>426</v>
+      </c>
+      <c r="F2" t="s">
+        <v>427</v>
+      </c>
+      <c r="G2" t="s">
+        <v>428</v>
+      </c>
+      <c r="H2" t="s">
+        <v>429</v>
+      </c>
+      <c r="I2" t="s">
+        <v>430</v>
+      </c>
+      <c r="J2" t="s">
+        <v>431</v>
+      </c>
+      <c r="K2" t="s">
+        <v>412</v>
+      </c>
+      <c r="L2" t="s">
+        <v>432</v>
+      </c>
+      <c r="M2" t="s">
+        <v>433</v>
+      </c>
+      <c r="N2" t="s">
+        <v>434</v>
+      </c>
+      <c r="O2" t="s">
+        <v>435</v>
+      </c>
+      <c r="P2" t="s">
+        <v>436</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B3" t="s">
+        <v>438</v>
+      </c>
+      <c r="C3" t="s">
+        <v>439</v>
+      </c>
+      <c r="D3" t="s">
+        <v>440</v>
+      </c>
+      <c r="E3" t="s">
+        <v>441</v>
+      </c>
+      <c r="F3" t="s">
+        <v>442</v>
+      </c>
+      <c r="G3" t="s">
+        <v>443</v>
+      </c>
+      <c r="H3" t="s">
+        <v>444</v>
+      </c>
+      <c r="I3" t="s">
+        <v>445</v>
+      </c>
+      <c r="J3" t="s">
+        <v>446</v>
+      </c>
+      <c r="K3" t="s">
+        <v>447</v>
+      </c>
+      <c r="L3" t="s">
+        <v>448</v>
+      </c>
+      <c r="M3" t="s">
+        <v>449</v>
+      </c>
+      <c r="N3" t="s">
+        <v>450</v>
+      </c>
+      <c r="O3" t="s">
+        <v>451</v>
+      </c>
+      <c r="P3" t="s">
+        <v>452</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>333</v>
+      </c>
+      <c r="B4" t="s">
+        <v>349</v>
+      </c>
+      <c r="C4" t="s">
+        <v>351</v>
+      </c>
+      <c r="D4" t="s">
+        <v>353</v>
+      </c>
+      <c r="E4" t="s">
+        <v>355</v>
+      </c>
+      <c r="F4" t="s">
+        <v>357</v>
+      </c>
+      <c r="G4" t="s">
+        <v>387</v>
+      </c>
+      <c r="H4" t="s">
+        <v>389</v>
+      </c>
+      <c r="I4" t="s">
+        <v>391</v>
+      </c>
+      <c r="J4" t="s">
+        <v>393</v>
+      </c>
+      <c r="K4" t="s">
+        <v>395</v>
+      </c>
+      <c r="L4" t="s">
+        <v>397</v>
+      </c>
+      <c r="M4" t="s">
+        <v>398</v>
+      </c>
+      <c r="N4" t="s">
+        <v>399</v>
+      </c>
+      <c r="O4" t="s">
+        <v>400</v>
+      </c>
+      <c r="P4" t="s">
+        <v>401</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>325</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D5" t="s">
+        <v>235</v>
+      </c>
+      <c r="E5" t="s">
+        <v>236</v>
+      </c>
+      <c r="F5" t="s">
+        <v>237</v>
+      </c>
+      <c r="G5" t="s">
+        <v>238</v>
+      </c>
+      <c r="H5" t="s">
+        <v>239</v>
+      </c>
+      <c r="I5" t="s">
+        <v>240</v>
+      </c>
+      <c r="J5" t="s">
+        <v>241</v>
+      </c>
+      <c r="K5" t="s">
+        <v>172</v>
+      </c>
+      <c r="L5" t="s">
+        <v>242</v>
+      </c>
+      <c r="M5" t="s">
+        <v>243</v>
+      </c>
+      <c r="N5" t="s">
+        <v>244</v>
+      </c>
+      <c r="O5" t="s">
+        <v>245</v>
+      </c>
+      <c r="P5" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>566</v>
+      </c>
+      <c r="C7" t="s">
+        <v>567</v>
+      </c>
+      <c r="D7" t="s">
+        <v>568</v>
+      </c>
+      <c r="E7" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>575</v>
+      </c>
+      <c r="D8" t="s">
+        <v>573</v>
+      </c>
+      <c r="E8" t="s">
+        <v>572</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394B7C90-4D65-4AFD-BE66-548D7075EB0B}">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F1" t="s">
+        <v>251</v>
+      </c>
+      <c r="G1" t="s">
+        <v>252</v>
+      </c>
+      <c r="H1" t="s">
+        <v>253</v>
+      </c>
+      <c r="I1" t="s">
+        <v>254</v>
+      </c>
+      <c r="J1" t="s">
+        <v>255</v>
+      </c>
+      <c r="K1" t="s">
+        <v>256</v>
+      </c>
+      <c r="L1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C2" t="s">
+        <v>352</v>
+      </c>
+      <c r="D2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E2" t="s">
+        <v>356</v>
+      </c>
+      <c r="F2" t="s">
+        <v>358</v>
+      </c>
+      <c r="G2" t="s">
+        <v>388</v>
+      </c>
+      <c r="H2" t="s">
+        <v>390</v>
+      </c>
+      <c r="I2" t="s">
+        <v>392</v>
+      </c>
+      <c r="J2" t="s">
+        <v>394</v>
+      </c>
+      <c r="K2" t="s">
+        <v>396</v>
+      </c>
+      <c r="L2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>332</v>
+      </c>
+      <c r="B3" t="s">
+        <v>456</v>
+      </c>
+      <c r="C3" t="s">
+        <v>457</v>
+      </c>
+      <c r="D3" t="s">
+        <v>458</v>
+      </c>
+      <c r="E3" t="s">
+        <v>459</v>
+      </c>
+      <c r="F3" t="s">
+        <v>460</v>
+      </c>
+      <c r="G3" t="s">
+        <v>461</v>
+      </c>
+      <c r="H3" t="s">
+        <v>462</v>
+      </c>
+      <c r="I3" t="s">
+        <v>463</v>
+      </c>
+      <c r="J3" t="s">
+        <v>402</v>
+      </c>
+      <c r="K3" t="s">
+        <v>464</v>
+      </c>
+      <c r="L3" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>333</v>
+      </c>
+      <c r="B4" t="s">
+        <v>424</v>
+      </c>
+      <c r="C4" t="s">
+        <v>425</v>
+      </c>
+      <c r="D4" t="s">
+        <v>426</v>
+      </c>
+      <c r="E4" t="s">
+        <v>427</v>
+      </c>
+      <c r="F4" t="s">
+        <v>428</v>
+      </c>
+      <c r="G4" t="s">
+        <v>429</v>
+      </c>
+      <c r="H4" t="s">
+        <v>430</v>
+      </c>
+      <c r="I4" t="s">
+        <v>431</v>
+      </c>
+      <c r="J4" t="s">
+        <v>412</v>
+      </c>
+      <c r="K4" t="s">
+        <v>432</v>
+      </c>
+      <c r="L4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>325</v>
+      </c>
+      <c r="B5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C5" t="s">
+        <v>303</v>
+      </c>
+      <c r="D5" t="s">
+        <v>304</v>
+      </c>
+      <c r="E5" t="s">
+        <v>305</v>
+      </c>
+      <c r="F5" t="s">
+        <v>306</v>
+      </c>
+      <c r="G5" t="s">
+        <v>307</v>
+      </c>
+      <c r="H5" t="s">
+        <v>308</v>
+      </c>
+      <c r="I5" t="s">
+        <v>309</v>
+      </c>
+      <c r="J5" t="s">
+        <v>310</v>
+      </c>
+      <c r="K5" t="s">
+        <v>311</v>
+      </c>
+      <c r="L5" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>566</v>
+      </c>
+      <c r="C7" t="s">
+        <v>567</v>
+      </c>
+      <c r="D7" t="s">
+        <v>568</v>
+      </c>
+      <c r="E7" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>575</v>
+      </c>
+      <c r="D8" t="s">
+        <v>574</v>
+      </c>
+      <c r="E8" t="s">
+        <v>572</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E3F9697-4688-4744-8455-559F4CBDA04E}">
+  <dimension ref="A1:AI6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D1" t="s">
+        <v>471</v>
+      </c>
+      <c r="E1" t="s">
+        <v>472</v>
+      </c>
+      <c r="F1" t="s">
+        <v>473</v>
+      </c>
+      <c r="G1" t="s">
+        <v>474</v>
+      </c>
+      <c r="H1" t="s">
+        <v>475</v>
+      </c>
+      <c r="I1" t="s">
+        <v>476</v>
+      </c>
+      <c r="J1" t="s">
+        <v>477</v>
+      </c>
+      <c r="K1" t="s">
+        <v>478</v>
+      </c>
+      <c r="L1" t="s">
+        <v>479</v>
+      </c>
+      <c r="M1" t="s">
+        <v>480</v>
+      </c>
+      <c r="N1" t="s">
+        <v>481</v>
+      </c>
+      <c r="O1" t="s">
+        <v>482</v>
+      </c>
+      <c r="P1" t="s">
+        <v>483</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>484</v>
+      </c>
+      <c r="R1" t="s">
+        <v>517</v>
+      </c>
+      <c r="S1" t="s">
+        <v>518</v>
+      </c>
+      <c r="T1" t="s">
+        <v>519</v>
+      </c>
+      <c r="U1" t="s">
+        <v>520</v>
+      </c>
+      <c r="V1" t="s">
+        <v>521</v>
+      </c>
+      <c r="W1" t="s">
+        <v>522</v>
+      </c>
+      <c r="X1" t="s">
+        <v>523</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>524</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>525</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>526</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>527</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>528</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>529</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>530</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>531</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>532</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>531</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B2" t="s">
+        <v>485</v>
+      </c>
+      <c r="C2" t="s">
+        <v>486</v>
+      </c>
+      <c r="D2" t="s">
+        <v>487</v>
+      </c>
+      <c r="E2" t="s">
+        <v>488</v>
+      </c>
+      <c r="F2" t="s">
+        <v>489</v>
+      </c>
+      <c r="G2" t="s">
+        <v>490</v>
+      </c>
+      <c r="H2" t="s">
+        <v>491</v>
+      </c>
+      <c r="I2" t="s">
+        <v>492</v>
+      </c>
+      <c r="J2" t="s">
+        <v>493</v>
+      </c>
+      <c r="K2" t="s">
+        <v>494</v>
+      </c>
+      <c r="L2" t="s">
+        <v>495</v>
+      </c>
+      <c r="M2" t="s">
+        <v>496</v>
+      </c>
+      <c r="N2" t="s">
+        <v>497</v>
+      </c>
+      <c r="O2" t="s">
+        <v>498</v>
+      </c>
+      <c r="P2" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>500</v>
+      </c>
+      <c r="R2" t="s">
+        <v>534</v>
+      </c>
+      <c r="S2" t="s">
+        <v>535</v>
+      </c>
+      <c r="T2" t="s">
+        <v>536</v>
+      </c>
+      <c r="U2" t="s">
+        <v>537</v>
+      </c>
+      <c r="V2" t="s">
+        <v>538</v>
+      </c>
+      <c r="W2" t="s">
+        <v>539</v>
+      </c>
+      <c r="X2" t="s">
+        <v>540</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>541</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>542</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>543</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>544</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>545</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>546</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>547</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>531</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>548</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>531</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>468</v>
+      </c>
+      <c r="B3" t="s">
+        <v>501</v>
+      </c>
+      <c r="C3" t="s">
+        <v>502</v>
+      </c>
+      <c r="D3" t="s">
+        <v>503</v>
+      </c>
+      <c r="E3" t="s">
+        <v>504</v>
+      </c>
+      <c r="F3" t="s">
+        <v>505</v>
+      </c>
+      <c r="G3" t="s">
+        <v>506</v>
+      </c>
+      <c r="H3" t="s">
+        <v>507</v>
+      </c>
+      <c r="I3" t="s">
+        <v>508</v>
+      </c>
+      <c r="J3" t="s">
+        <v>509</v>
+      </c>
+      <c r="K3" t="s">
+        <v>510</v>
+      </c>
+      <c r="L3" t="s">
+        <v>511</v>
+      </c>
+      <c r="M3" t="s">
+        <v>512</v>
+      </c>
+      <c r="N3" t="s">
+        <v>513</v>
+      </c>
+      <c r="O3" t="s">
+        <v>514</v>
+      </c>
+      <c r="P3" t="s">
+        <v>515</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>516</v>
+      </c>
+      <c r="R3" t="s">
+        <v>550</v>
+      </c>
+      <c r="S3" t="s">
+        <v>551</v>
+      </c>
+      <c r="T3" t="s">
+        <v>552</v>
+      </c>
+      <c r="U3" t="s">
+        <v>553</v>
+      </c>
+      <c r="V3" t="s">
+        <v>554</v>
+      </c>
+      <c r="W3" t="s">
+        <v>555</v>
+      </c>
+      <c r="X3" t="s">
+        <v>556</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>557</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>558</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>559</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>560</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>561</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>562</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>563</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>531</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>564</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>531</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>566</v>
+      </c>
+      <c r="C5" t="s">
+        <v>567</v>
+      </c>
+      <c r="D5" t="s">
+        <v>568</v>
+      </c>
+      <c r="E5" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>576</v>
+      </c>
+      <c r="D6" t="s">
+        <v>571</v>
+      </c>
+      <c r="E6" t="s">
+        <v>577</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C77CEBB-BA59-4E76-B575-E17059FB5FF7}">
+  <dimension ref="A1:Q6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B1" t="s">
+        <v>474</v>
+      </c>
+      <c r="C1" t="s">
+        <v>476</v>
+      </c>
+      <c r="D1" t="s">
+        <v>478</v>
+      </c>
+      <c r="E1" t="s">
+        <v>480</v>
+      </c>
+      <c r="F1" t="s">
+        <v>482</v>
+      </c>
+      <c r="G1" t="s">
+        <v>484</v>
+      </c>
+      <c r="H1" t="s">
+        <v>518</v>
+      </c>
+      <c r="I1" t="s">
+        <v>520</v>
+      </c>
+      <c r="J1" t="s">
+        <v>522</v>
+      </c>
+      <c r="K1" t="s">
+        <v>524</v>
+      </c>
+      <c r="L1" t="s">
+        <v>526</v>
+      </c>
+      <c r="M1" t="s">
+        <v>528</v>
+      </c>
+      <c r="N1" t="s">
+        <v>529</v>
+      </c>
+      <c r="O1" t="s">
+        <v>530</v>
+      </c>
+      <c r="P1" t="s">
+        <v>532</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B2" t="s">
+        <v>490</v>
+      </c>
+      <c r="C2" t="s">
+        <v>492</v>
+      </c>
+      <c r="D2" t="s">
+        <v>494</v>
+      </c>
+      <c r="E2" t="s">
+        <v>496</v>
+      </c>
+      <c r="F2" t="s">
+        <v>498</v>
+      </c>
+      <c r="G2" t="s">
+        <v>500</v>
+      </c>
+      <c r="H2" t="s">
+        <v>535</v>
+      </c>
+      <c r="I2" t="s">
+        <v>537</v>
+      </c>
+      <c r="J2" t="s">
+        <v>539</v>
+      </c>
+      <c r="K2" t="s">
+        <v>541</v>
+      </c>
+      <c r="L2" t="s">
+        <v>543</v>
+      </c>
+      <c r="M2" t="s">
+        <v>545</v>
+      </c>
+      <c r="N2" t="s">
+        <v>546</v>
+      </c>
+      <c r="O2" t="s">
+        <v>547</v>
+      </c>
+      <c r="P2" t="s">
+        <v>548</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>468</v>
+      </c>
+      <c r="B3" t="s">
+        <v>506</v>
+      </c>
+      <c r="C3" t="s">
+        <v>508</v>
+      </c>
+      <c r="D3" t="s">
+        <v>510</v>
+      </c>
+      <c r="E3" t="s">
+        <v>512</v>
+      </c>
+      <c r="F3" t="s">
+        <v>514</v>
+      </c>
+      <c r="G3" t="s">
+        <v>516</v>
+      </c>
+      <c r="H3" t="s">
+        <v>551</v>
+      </c>
+      <c r="I3" t="s">
+        <v>553</v>
+      </c>
+      <c r="J3" t="s">
+        <v>555</v>
+      </c>
+      <c r="K3" t="s">
+        <v>557</v>
+      </c>
+      <c r="L3" t="s">
+        <v>559</v>
+      </c>
+      <c r="M3" t="s">
+        <v>561</v>
+      </c>
+      <c r="N3" t="s">
+        <v>562</v>
+      </c>
+      <c r="O3" t="s">
+        <v>563</v>
+      </c>
+      <c r="P3" t="s">
+        <v>564</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>566</v>
+      </c>
+      <c r="C5" t="s">
+        <v>567</v>
+      </c>
+      <c r="D5" t="s">
+        <v>568</v>
+      </c>
+      <c r="E5" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>576</v>
+      </c>
+      <c r="D6" t="s">
+        <v>573</v>
+      </c>
+      <c r="E6" t="s">
+        <v>578</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BDC86FC-D89D-4BB7-8577-F8DA59F2D90D}">
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B1" t="s">
+        <v>581</v>
+      </c>
+      <c r="C1" t="s">
+        <v>582</v>
+      </c>
+      <c r="D1" t="s">
+        <v>583</v>
+      </c>
+      <c r="E1" t="s">
+        <v>504</v>
+      </c>
+      <c r="F1" t="s">
+        <v>584</v>
+      </c>
+      <c r="G1" t="s">
+        <v>585</v>
+      </c>
+      <c r="H1" t="s">
+        <v>586</v>
+      </c>
+      <c r="I1" t="s">
+        <v>587</v>
+      </c>
+      <c r="J1" t="s">
+        <v>588</v>
+      </c>
+      <c r="K1" t="s">
+        <v>589</v>
+      </c>
+      <c r="L1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B2" t="s">
+        <v>590</v>
+      </c>
+      <c r="C2" t="s">
+        <v>591</v>
+      </c>
+      <c r="D2" t="s">
+        <v>592</v>
+      </c>
+      <c r="E2" t="s">
+        <v>593</v>
+      </c>
+      <c r="F2" t="s">
+        <v>594</v>
+      </c>
+      <c r="G2" t="s">
+        <v>595</v>
+      </c>
+      <c r="H2" t="s">
+        <v>596</v>
+      </c>
+      <c r="I2" t="s">
+        <v>597</v>
+      </c>
+      <c r="J2" t="s">
+        <v>598</v>
+      </c>
+      <c r="K2" t="s">
+        <v>599</v>
+      </c>
+      <c r="L2" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>580</v>
+      </c>
+      <c r="B3" t="s">
+        <v>582</v>
+      </c>
+      <c r="C3" t="s">
+        <v>583</v>
+      </c>
+      <c r="D3" t="s">
+        <v>504</v>
+      </c>
+      <c r="E3" t="s">
+        <v>584</v>
+      </c>
+      <c r="F3" t="s">
+        <v>585</v>
+      </c>
+      <c r="G3" t="s">
+        <v>600</v>
+      </c>
+      <c r="H3" t="s">
+        <v>601</v>
+      </c>
+      <c r="I3" t="s">
+        <v>588</v>
+      </c>
+      <c r="J3" t="s">
+        <v>589</v>
+      </c>
+      <c r="K3" t="s">
+        <v>602</v>
+      </c>
+      <c r="L3" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>466</v>
+      </c>
+      <c r="B4" t="s">
+        <v>603</v>
+      </c>
+      <c r="C4" t="s">
+        <v>604</v>
+      </c>
+      <c r="D4" t="s">
+        <v>605</v>
+      </c>
+      <c r="E4" t="s">
+        <v>606</v>
+      </c>
+      <c r="F4" t="s">
+        <v>607</v>
+      </c>
+      <c r="G4" t="s">
+        <v>608</v>
+      </c>
+      <c r="H4" t="s">
+        <v>609</v>
+      </c>
+      <c r="I4" t="s">
+        <v>610</v>
+      </c>
+      <c r="J4" t="s">
+        <v>611</v>
+      </c>
+      <c r="K4" t="s">
+        <v>612</v>
+      </c>
+      <c r="L4" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>566</v>
+      </c>
+      <c r="C6" t="s">
+        <v>567</v>
+      </c>
+      <c r="D6" t="s">
+        <v>568</v>
+      </c>
+      <c r="E6" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>617</v>
+      </c>
+      <c r="D7" t="s">
+        <v>571</v>
+      </c>
+      <c r="E7" t="s">
+        <v>577</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dev build 0.365 (buses for fast-travel)
- Added bus graphics.
- Some updates to the Tiled map.
</commit_message>
<xml_diff>
--- a/data/bus_data.xlsx
+++ b/data/bus_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/efc7ce48255d0cb5/Documents/2023 S2/COSC345/COSC345-Game/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas Pedersen\Documents\GitHub\COSC345-Game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="8_{92D09202-F985-4960-AFF2-A8F234A16CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80325E16-2F38-482A-A44E-F790A87982D1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1AA0A3-6848-4F51-8F89-2F734B4BBB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="9" xr2:uid="{08F58157-5B37-470B-8714-523729044959}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{08F58157-5B37-470B-8714-523729044959}"/>
   </bookViews>
   <sheets>
     <sheet name="15N M-F" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="674">
   <si>
     <t>5:50am</t>
   </si>
@@ -2058,6 +2058,15 @@
   </si>
   <si>
     <t>12:05a.m.</t>
+  </si>
+  <si>
+    <t>Departure 1</t>
+  </si>
+  <si>
+    <t>Departure 2</t>
+  </si>
+  <si>
+    <t>and so on</t>
   </si>
 </sst>
 </file>
@@ -2113,7 +2122,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2401,7 +2410,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2409,18 +2418,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D2E1A5-2446-445B-A24B-7B29F9CDA543}">
-  <dimension ref="A1:AF9"/>
+  <dimension ref="A1:AF13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>325</v>
       </c>
@@ -2518,7 +2527,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>326</v>
       </c>
@@ -2616,7 +2625,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>327</v>
       </c>
@@ -2714,7 +2723,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>328</v>
       </c>
@@ -2812,7 +2821,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>329</v>
       </c>
@@ -2910,7 +2919,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>330</v>
       </c>
@@ -3008,7 +3017,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>566</v>
       </c>
@@ -3022,7 +3031,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>15</v>
       </c>
@@ -3034,6 +3043,69 @@
       </c>
       <c r="E9" t="s">
         <v>572</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>671</v>
+      </c>
+      <c r="B11" t="str">
+        <f>B1</f>
+        <v>5:50am</v>
+      </c>
+      <c r="C11" t="str">
+        <f>B2</f>
+        <v>5:53am</v>
+      </c>
+      <c r="D11" t="str">
+        <f>B3</f>
+        <v>6:01am</v>
+      </c>
+      <c r="E11" t="str">
+        <f>B4</f>
+        <v>6:07am</v>
+      </c>
+      <c r="F11" t="str">
+        <f>B5</f>
+        <v>6:18am</v>
+      </c>
+      <c r="G11" t="str">
+        <f>B6</f>
+        <v>6:25am</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>672</v>
+      </c>
+      <c r="B12" t="str">
+        <f>C1</f>
+        <v>6:10am</v>
+      </c>
+      <c r="C12" t="str">
+        <f>C2</f>
+        <v>6:13am</v>
+      </c>
+      <c r="D12" t="str">
+        <f>C3</f>
+        <v>6:21am</v>
+      </c>
+      <c r="E12" t="str">
+        <f>C4</f>
+        <v>6:27am</v>
+      </c>
+      <c r="F12" t="str">
+        <f>C5</f>
+        <v>6:38am</v>
+      </c>
+      <c r="G12" t="str">
+        <f>C6</f>
+        <v>6:45am</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>673</v>
       </c>
     </row>
   </sheetData>
@@ -3045,16 +3117,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27BA5E9F-3C21-4944-A859-C18E0E66A19E}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>579</v>
       </c>
@@ -3107,7 +3179,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>467</v>
       </c>
@@ -3160,7 +3232,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>580</v>
       </c>
@@ -3213,7 +3285,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>466</v>
       </c>
@@ -3266,7 +3338,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>566</v>
       </c>
@@ -3280,7 +3352,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>14</v>
       </c>
@@ -3307,12 +3379,12 @@
       <selection activeCell="B8" sqref="B8:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>325</v>
       </c>
@@ -3365,7 +3437,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>326</v>
       </c>
@@ -3418,7 +3490,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>327</v>
       </c>
@@ -3471,7 +3543,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>328</v>
       </c>
@@ -3524,7 +3596,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>329</v>
       </c>
@@ -3577,7 +3649,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>330</v>
       </c>
@@ -3630,7 +3702,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>566</v>
       </c>
@@ -3644,7 +3716,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>15</v>
       </c>
@@ -3671,12 +3743,12 @@
       <selection activeCell="B8" sqref="B8:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>325</v>
       </c>
@@ -3714,7 +3786,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>326</v>
       </c>
@@ -3752,7 +3824,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>327</v>
       </c>
@@ -3790,7 +3862,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>328</v>
       </c>
@@ -3828,7 +3900,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>329</v>
       </c>
@@ -3866,7 +3938,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>330</v>
       </c>
@@ -3904,7 +3976,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>566</v>
       </c>
@@ -3918,7 +3990,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>15</v>
       </c>
@@ -3945,12 +4017,12 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>330</v>
       </c>
@@ -4045,7 +4117,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>331</v>
       </c>
@@ -4140,7 +4212,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>332</v>
       </c>
@@ -4235,7 +4307,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>333</v>
       </c>
@@ -4330,7 +4402,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>325</v>
       </c>
@@ -4425,7 +4497,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>566</v>
       </c>
@@ -4439,7 +4511,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>15</v>
       </c>
@@ -4469,12 +4541,12 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>330</v>
       </c>
@@ -4527,7 +4599,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>331</v>
       </c>
@@ -4580,7 +4652,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>332</v>
       </c>
@@ -4633,7 +4705,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>333</v>
       </c>
@@ -4686,7 +4758,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>325</v>
       </c>
@@ -4739,7 +4811,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>566</v>
       </c>
@@ -4753,7 +4825,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>15</v>
       </c>
@@ -4780,12 +4852,12 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>330</v>
       </c>
@@ -4823,7 +4895,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>331</v>
       </c>
@@ -4861,7 +4933,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>332</v>
       </c>
@@ -4899,7 +4971,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>333</v>
       </c>
@@ -4937,7 +5009,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>325</v>
       </c>
@@ -4975,7 +5047,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>566</v>
       </c>
@@ -4989,7 +5061,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>15</v>
       </c>
@@ -5016,12 +5088,12 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>466</v>
       </c>
@@ -5128,7 +5200,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>467</v>
       </c>
@@ -5235,7 +5307,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>468</v>
       </c>
@@ -5342,7 +5414,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>566</v>
       </c>
@@ -5356,7 +5428,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>14</v>
       </c>
@@ -5383,12 +5455,12 @@
       <selection activeCell="B5" sqref="B5:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>466</v>
       </c>
@@ -5441,7 +5513,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>467</v>
       </c>
@@ -5494,7 +5566,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>468</v>
       </c>
@@ -5547,7 +5619,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>566</v>
       </c>
@@ -5561,7 +5633,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>14</v>
       </c>
@@ -5588,12 +5660,12 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>579</v>
       </c>
@@ -5631,7 +5703,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>467</v>
       </c>
@@ -5669,7 +5741,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>580</v>
       </c>
@@ -5707,7 +5779,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>466</v>
       </c>
@@ -5745,7 +5817,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>566</v>
       </c>
@@ -5759,7 +5831,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Update final sheet with 77 summary
</commit_message>
<xml_diff>
--- a/data/bus_data.xlsx
+++ b/data/bus_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/efc7ce48255d0cb5/Documents/2023 S2/COSC345/COSC345-Game/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{8EDDDD44-A2BC-4C76-A3DD-24A0FFC4D2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="14_{8EDDDD44-A2BC-4C76-A3DD-24A0FFC4D2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4865BFDF-1D69-4E48-9C4D-4F29A83956A2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="19" activeTab="29" xr2:uid="{08F58157-5B37-470B-8714-523729044959}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6511" uniqueCount="993">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6529" uniqueCount="1004">
   <si>
     <t>5:50am</t>
   </si>
@@ -3044,6 +3044,39 @@
   </si>
   <si>
     <t>Departure 1,8:38am,9:01am,9:04am,9:10am,9:19am,Departure 2,9:38am,10:01am,10:04am,10:10am,10:19am,Departure 3,10:38am,11:01am,11:04am,11:10am,11:19am,Departure 4,11:38am,12:01pm,12:04pm,12:10pm,12:19pm,Departure 5,12:38pm,1:01pm,1:04pm,1:10pm,1:19pm,Departure 6,1:38pm,2:01pm,2:04pm,2:10pm,2:19pm,Departure 7,2:38pm,3:01pm,3:04pm,3:10pm,3:19pm,Departure 8,3:38pm,4:01pm,4:04pm,4:10pm,4:19pm,Departure 9,4:38pm,5:01pm,5:04pm,5:10pm,5:19pm,Departure 10,5:38pm,6:01pm,6:04pm,6:10pm,6:19pm,Departure 11,6:38pm,7:01pm,7:04pm,7:10pm,7:19pm,Departure 12,7:38pm,8:01pm,8:04pm,8:10pm,8:19pm,Departure 13,8:38pm,9:01pm,9:04pm,9:10pm,9:19pm</t>
+  </si>
+  <si>
+    <t>Mosgiel Terminus;Fairfield, cnr Fairplay St;Green Is. (Inbound);Bus Hub Stop F</t>
+  </si>
+  <si>
+    <t>Departure 1,6:00am,6:15am,6:20am,6:37am,Departure 2,6:30am,6:45am,6:50am,7:07am,Departure 3,7:00am,7:15am,7:20am,7:37am,Departure 4,7:15am,7:30am,7:35am,7:52am,Departure 5,7:30am,7:45am,7:50am,8:07am,Departure 6,7:45am,8:00am,8:05am,8:22am,Departure 7,8:00am,8:15am,8:20am,8:37am,Departure 8,8:15am,8:30am,8:35am,8:52am,Departure 9,8:30am,8:45am,8:50am,9:07am,Departure 10,8:45am,9:00am,9:05am,9:22am,Departure 11,9:00am,9:15am,9:20am,9:37am,Departure 12,9:30am,9:45am,9:50am,10:07am,Departure 13,10:00am,10:15am,10:20am,10:37am,Departure 14,10:30am,10:45am,10:50am,11:07am,Departure 15,11:00am,11:15am,11:20am,11:37am,Departure 16,11:30am,11:45am,11:50am,12:07pm,Departure 17,12:00pm,12:15pm,12:20pm,12:37pm,Departure 18,12:30pm,12:45pm,12:50pm,1:07pm,Departure 19,1:00pm,1:15pm,1:20pm,1:37pm,Departure 20,1:30pm,1:45pm,1:50pm,2:07pm,Departure 21,2:00pm,2:15pm,2:20pm,2:37pm,Departure 22,2:30pm,2:45pm,2:50pm,3:07pm,Departure 23,3:00pm,3:15pm,3:20pm,3:37pm,Departure 24,3:15pm,3:30pm,3:35pm,3:52pm,Departure 25,3:30pm,3:45pm,3:50pm,4:07pm,Departure 26,3:45pm,4:00pm,4:05pm,4:22pm,Departure 27,4:00pm,4:15pm,4:20pm,4:37pm,Departure 28,4:15pm,4:30pm,4:35pm,4:52pm,Departure 29,4:30pm,4:45pm,4:50pm,5:07pm,Departure 30,4:45pm,5:00pm,5:05pm,5:22pm,Departure 31,5:00pm,5:15pm,5:20pm,5:37pm,Departure 32,5:30pm,5:45pm,5:50pm,6:07pm,Departure 33,6:00pm,6:15pm,6:20pm,6:37pm,Departure 34,6:30pm,6:45pm,6:50pm,7:07pm,Departure 35,7:30pm,7:45pm,7:50pm,8:07pm,Departure 36,8:00pm,8:15pm,8:20pm,8:37pm</t>
+  </si>
+  <si>
+    <t>77M</t>
+  </si>
+  <si>
+    <t>Departure 1,8:00am,8:00am,8:15am,8:20am,8:37am,Departure 2,8:30am,8:30am,8:45am,8:50am,9:07am,Departure 3,9:00am,9:00am,9:15am,9:20am,9:37am,Departure 4,9:30am,9:30am,9:45am,9:50am,10:07am,Departure 5,10:00am,10:00am,10:15am,10:20am,10:37am,Departure 6,10:30am,10:30am,10:45am,10:50am,11:07am,Departure 7,11:00am,11:00am,11:15am,11:20am,11:37am,Departure 8,11:30am,11:30am,11:45am,11:50am,12:07pm,Departure 9,12:00pm,12:00pm,12:15pm,12:20pm,12:37pm,Departure 10,12:30pm,12:30pm,12:45pm,12:50pm,1:07pm,Departure 11,1:00pm,1:00pm,1:15pm,1:20pm,1:37pm,Departure 12,1:30pm,1:30pm,1:45pm,1:50pm,2:07pm,Departure 13,2:00pm,2:00pm,2:15pm,2:20pm,2:37pm,Departure 14,2:30pm,2:30pm,2:45pm,2:50pm,3:07pm,Departure 15,3:00pm,3:00pm,3:15pm,3:20pm,3:37pm,Departure 16,3:30pm,3:30pm,3:45pm,3:50pm,4:07pm,Departure 17,4:00pm,4:00pm,4:15pm,4:20pm,4:37pm,Departure 18,4:30pm,4:30pm,4:45pm,4:50pm,5:07pm,Departure 19,5:30pm,5:30pm,5:45pm,5:50pm,6:07pm,Departure 20,7:30pm,7:30pm,7:45pm,7:50pm,8:07pm,Departure 21,9:00pm,9:00pm,9:15pm,9:20pm,9:37pm,Departure 22,10:30pm,10:30pm,10:45pm,10:50pm,11:07pm</t>
+  </si>
+  <si>
+    <t>Departure 1,8:00am,8:00am,8:15am,8:20am,8:37am,Departure 2,8:30am,8:30am,8:45am,8:50am,9:07am,Departure 3,9:00am,9:00am,9:15am,9:20am,9:37am,Departure 4,9:30am,9:30am,9:45am,9:50am,10:07am,Departure 5,10:00am,10:00am,10:15am,10:20am,10:37am,Departure 6,10:30am,10:30am,10:45am,10:50am,11:07am,Departure 7,11:00am,11:00am,11:15am,11:20am,11:37am,Departure 8,11:30am,11:30am,11:45am,11:50am,12:07pm,Departure 9,12:00pm,12:00pm,12:15pm,12:20pm,12:37pm,Departure 10,12:30pm,12:30pm,12:45pm,12:50pm,1:07pm,Departure 11,1:00pm,1:00pm,1:15pm,1:20pm,1:37pm,Departure 12,1:30pm,1:30pm,1:45pm,1:50pm,2:07pm,Departure 13,2:00pm,2:00pm,2:15pm,2:20pm,2:37pm,Departure 14,2:30pm,2:30pm,2:45pm,2:50pm,3:07pm,Departure 15,3:00pm,3:00pm,3:15pm,3:20pm,3:37pm,Departure 16,3:30pm,3:30pm,3:45pm,3:50pm,4:07pm,Departure 17,4:00pm,4:00pm,4:15pm,4:20pm,4:37pm,Departure 18,4:30pm,4:30pm,4:45pm,4:50pm,5:07pm,Departure 19,5:30pm,5:30pm,5:45pm,5:50pm,6:07pm,Departure 20,7:30pm,7:30pm,7:45pm,7:50pm,8:07pm,Departure 21,9:00pm,9:00pm,9:15pm,9:20pm,9:37pm</t>
+  </si>
+  <si>
+    <t>77C</t>
+  </si>
+  <si>
+    <t>Bus Hub Stop F;Green Is. (Outbound);Morris Rd, cnr Coach Rd;Mosgiel Terminus</t>
+  </si>
+  <si>
+    <t>Departure 1,7:12am,7:29am,7:35am,7:50am,Departure 2,7:42am,7:59am,8:05am,8:20am,Departure 3,7:57am,8:14am,8:20am,8:35am,Departure 4,8:12am,8:29am,8:35am,8:50am,Departure 5,8:27am,8:44am,8:50am,9:05am,Departure 6,8:42am,8:59am,9:05am,9:20am,Departure 7,8:57am,9:14am,9:20am,9:35am,Departure 8,9:12am,9:29am,9:35am,9:50am,Departure 9,9:42am,9:59am,10:05am,10:20am,Departure 10,10:12am,10:29am,10:35am,10:50am,Departure 11,10:42am,10:59am,11:05am,11:20am,Departure 12,11:12am,11:29am,11:35am,11:50am,Departure 13,11:42am,11:59am,12:05pm,12:20pm,Departure 14,12:12pm,12:29pm,12:35pm,12:50pm,Departure 15,12:42pm,12:59pm,1:05pm,1:20pm,Departure 16,1:12pm,1:29pm,1:35pm,1:50pm,Departure 17,1:42pm,1:59pm,2:05pm,2:20pm,Departure 18,2:12pm,2:29pm,2:35pm,2:50pm,Departure 19,2:42pm,2:59pm,3:05pm,3:20pm,Departure 20,3:12pm,3:29pm,3:35pm,3:50pm,Departure 21,3:42pm,3:59pm,4:05pm,4:20pm,Departure 22,3:57pm,4:14pm,4:20pm,4:35pm,Departure 23,4:12pm,4:29pm,4:35pm,4:50pm,Departure 24,4:27pm,4:44pm,4:50pm,5:05pm,Departure 25,4:42pm,4:59pm,5:05pm,5:20pm,Departure 26,4:57pm,5:14pm,5:20pm,5:35pm,Departure 27,5:12pm,5:29pm,5:35pm,5:50pm,Departure 28,5:27pm,5:44pm,5:50pm,6:05pm,Departure 29,5:42pm,5:59pm,6:05pm,6:20pm,Departure 30,6:12pm,6:29pm,6:35pm,6:50pm,Departure 31,6:42pm,6:59pm,7:05pm,7:20pm,Departure 32,7:12pm,7:29pm,7:35pm,7:50pm,Departure 33,8:42pm,8:59pm,9:05pm,9:20pm</t>
+  </si>
+  <si>
+    <t>Departure 1,7:12am,7:29am,7:35am,7:50am,Departure 2,7:42am,7:59am,8:05am,8:20am,Departure 3,7:57am,8:14am,8:20am,8:35am,Departure 4,8:12am,8:29am,8:35am,8:50am,Departure 5,8:27am,8:44am,8:50am,9:05am,Departure 6,8:42am,8:59am,9:05am,9:20am,Departure 7,8:57am,9:14am,9:20am,9:35am,Departure 8,9:12am,9:29am,9:35am,9:50am,Departure 9,9:42am,9:59am,10:05am,10:20am,Departure 10,10:12am,10:29am,10:35am,10:50am,Departure 11,10:42am,10:59am,11:05am,11:20am,Departure 12,11:12am,11:29am,11:35am,11:50am,Departure 13,11:42am,11:59am,12:05pm,12:20pm,Departure 14,12:12pm,12:29pm,12:35pm,12:50pm,Departure 15,12:42pm,12:59pm,1:05pm,1:20pm,Departure 16,1:12pm,1:29pm,1:35pm,1:50pm,Departure 17,1:42pm,1:59pm,2:05pm,2:20pm,Departure 18,2:12pm,2:29pm,2:35pm,2:50pm,Departure 19,2:42pm,2:59pm,3:05pm,3:20pm,Departure 20,3:12pm,3:29pm,3:35pm,3:50pm,Departure 21,3:42pm,3:59pm,4:05pm,4:20pm,Departure 22,3:57pm,4:14pm,4:20pm,4:35pm,Departure 23,4:12pm,4:29pm,4:35pm,4:50pm,Departure 24,4:27pm,4:44pm,4:50pm,5:05pm,Departure 25,4:42pm,4:59pm,5:05pm,5:20pm,Departure 26,4:57pm,5:14pm,5:20pm,5:35pm,Departure 27,5:12pm,5:29pm,5:35pm,5:50pm,Departure 28,5:27pm,5:44pm,5:50pm,6:05pm,Departure 29,5:42pm,5:59pm,6:05pm,6:20pm,Departure 30,6:12pm,6:29pm,6:35pm,6:50pm,Departure 31,6:42pm,6:59pm,7:05pm,7:20pm,Departure 32,7:12pm,7:29pm,7:35pm,7:50pm,Departure 33,8:42pm,8:59pm,9:05pm,9:20pm,Departure 34,11:42pm,11:59pm,12:05am,12:20am</t>
+  </si>
+  <si>
+    <t>Departure 1,8:42am,8:59am,9:05am,9:20am,Departure 2,9:12am,9:29am,9:35am,9:50am,Departure 3,9:42am,9:59am,10:05am,10:20am,Departure 4,10:12am,10:29am,10:35am,10:50am,Departure 5,10:42am,10:59am,11:05am,11:20am,Departure 6,11:12am,11:29am,11:35am,11:50am,Departure 7,11:42am,11:59am,12:05pm,12:20pm,Departure 8,12:12pm,12:29pm,12:35pm,12:50pm,Departure 9,12:42pm,12:59pm,1:05pm,1:20pm,Departure 10,1:12pm,1:29pm,1:35pm,1:50pm,Departure 11,1:42pm,1:59pm,2:05pm,2:20pm,Departure 12,2:12pm,2:29pm,2:35pm,2:50pm,Departure 13,2:42pm,2:59pm,3:05pm,3:20pm,Departure 14,3:12pm,3:29pm,3:35pm,3:50pm,Departure 15,3:42pm,3:59pm,4:05pm,4:20pm,Departure 16,4:42pm,4:59pm,5:05pm,5:20pm,Departure 17,6:12pm,6:29pm,6:35pm,6:50pm,Departure 18,8:12pm,8:29pm,8:35pm,8:50pm,Departure 19,9:42pm,9:59pm,10:05pm,10:20pm,Departure 20,11:42pm,11:59pm,12:05am,12:20am</t>
+  </si>
+  <si>
+    <t>Departure 1,8:42am,8:59am,9:05am,9:20am,Departure 2,9:12am,9:29am,9:35am,9:50am,Departure 3,9:42am,9:59am,10:05am,10:20am,Departure 4,10:12am,10:29am,10:35am,10:50am,Departure 5,10:42am,10:59am,11:05am,11:20am,Departure 6,11:12am,11:29am,11:35am,11:50am,Departure 7,11:42am,11:59am,12:05pm,12:20pm,Departure 8,12:12pm,12:29pm,12:35pm,12:50pm,Departure 9,12:42pm,12:59pm,1:05pm,1:20pm,Departure 10,1:12pm,1:29pm,1:35pm,1:50pm,Departure 11,1:42pm,1:59pm,2:05pm,2:20pm,Departure 12,2:12pm,2:29pm,2:35pm,2:50pm,Departure 13,2:42pm,2:59pm,3:05pm,3:20pm,Departure 14,3:12pm,3:29pm,3:35pm,3:50pm,Departure 15,3:42pm,3:59pm,4:05pm,4:20pm,Departure 16,4:42pm,4:59pm,5:05pm,5:20pm,Departure 17,6:12pm,6:29pm,6:35pm,6:50pm,Departure 18,8:12pm,8:29pm,8:35pm,8:50pm,Departure 19,9:42pm,9:59pm,10:05pm,10:20pm</t>
   </si>
 </sst>
 </file>
@@ -3102,6 +3135,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14553,7 +14590,7 @@
   <dimension ref="A1:AK44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:G10"/>
+      <selection activeCell="G8" sqref="G8:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16449,7 +16486,7 @@
   <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17191,7 +17228,7 @@
   <dimension ref="A1:AH41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="A1:XFD1048576"/>
+      <selection activeCell="G8" sqref="G8:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18225,7 +18262,7 @@
   <dimension ref="A1:AI42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18687,12 +18724,6 @@
       </c>
       <c r="E7" t="s">
         <v>569</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="G8" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN('15S M-F'!G9, TRUE,A1:A4)</f>
-        <v>Bus Hub Stop F;Green Is. (Outbound);Morris Rd, cnr Coach Rd;Mosgiel Terminus</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.3">
@@ -19288,7 +19319,7 @@
   <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G9" sqref="A1:XFD1048576"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19939,7 +19970,7 @@
   <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21134,10 +21165,10 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8132FC2C-AE6B-4772-BB98-C781CEFEC7E4}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21145,7 +21176,7 @@
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>_xlfn.TEXTJOIN(A2, TRUE, B1:B1003)</f>
-        <v>271 Andersons Bay Rd;169 Hillside Rd;2 Mailer St;271 Highgate;Great King St North Botanic Gardens;Forth St Leith Bridge;Departure 1,5:50am,5:53am,6:01am,6:07am,6:18am,6:25am,Departure 2,6:10am,6:13am,6:21am,6:27am,6:38am,6:45am,Departure 3,6:40am,6:43am,6:51am,6:57am,7:08am,7:15am,Departure 4,7:10am,7:13am,7:21am,7:27am,7:38am,7:45am,Departure 5,7:40am,7:43am,7:53am,7:59am,8:12am,8:20am,Departure 6,8:10am,8:13am,8:23am,8:29am,8:42am,8:50am,Departure 7,8:40am,8:43am,8:51am,8:57am,9:08am,9:15am,Departure 8,9:10am,9:13am,9:21am,9:27am,9:38am,9:45am,Departure 9,9:40am,9:43am,9:51am,9:57am,10:08am,10:15am,Departure 10,10:10am,10:13am,10:21am,10:27am,10:38am,10:45am,Departure 11,10:40am,10:43am,10:51am,10:57am,11:08am,11:15am,Departure 12,11:10am,11:13am,11:21am,11:27am,11:38am,11:45am,Departure 13,11:40am,11:43am,11:51am,11:57am,12:08pm,12:15pm,Departure 14,12:10pm,12:13pm,12:21pm,12:27pm,12:38pm,12:45pm,Departure 15,12:40pm,12:43pm,12:51pm,12:57pm,1:08pm,1:15pm,Departure 16,1:10pm,1:13pm,1:21pm,1:27pm,1:38pm,1:45pm,Departure 17,1:40pm,1:43pm,1:51pm,1:57pm,2:08pm,2:15pm,Departure 18,2:10pm,2:13pm,2:21pm,2:27pm,2:38pm,2:45pm,Departure 19,2:40pm,2:43pm,2:51pm,2:57pm,3:08pm,3:15pm,Departure 20,3:10pm,3:13pm,3:21pm,3:27pm,3:38pm,3:45pm,Departure 21,3:40pm,3:43pm,3:51pm,3:57pm,4:08pm,4:15pm,Departure 22,4:10pm,4:13pm,4:21pm,4:27pm,4:38pm,4:45pm,Departure 23,4:40pm,4:43pm,4:51pm,4:57pm,5:08pm,5:15pm,Departure 24,5:10pm,5:13pm,5:23pm,5:29pm,5:42pm,5:50pm,Departure 25,5:40pm,5:43pm,5:53pm,5:59pm,6:12pm,6:20pm,Departure 26,6:10pm,6:13pm,6:21pm,6:27pm,6:38pm,6:45pm,Departure 27,6:40pm,6:43pm,6:51pm,6:57pm,7:08pm,7:15pm,Departure 28,7:30pm,7:33pm,7:41pm,7:47pm,7:58pm,8:05pm,Departure 29,8:30pm,8:33pm,8:41pm,8:47pm,8:58pm,9:05pm,Departure 30,9:30pm,9:33pm,9:41pm,9:47pm,9:58pm,10:05pm,Departure 31,10:30pm,10:33pm,10:41pm,10:47pm,10:58pm,11:05pm,;Departure 1,8:15am,8:18am,8:26am,8:32am,8:43am,8:50am,Departure 2,9:15am,9:18am,9:26am,9:32am,9:43am,9:50am,Departure 3,10:15am,10:18am,10:26am,10:32am,10:43am,10:50am,Departure 4,11:15am,11:18am,11:26am,11:32am,11:43am,11:50am,Departure 5,12:15pm,12:18pm,12:26pm,12:32pm,12:43pm,12:50pm,Departure 6,1:15pm,1:18pm,1:26pm,1:32pm,1:43pm,1:50pm,Departure 7,2:15pm,2:18pm,2:26pm,2:32pm,2:43pm,2:50pm,Departure 8,3:15pm,3:18pm,3:26pm,3:32pm,3:43pm,3:50pm,Departure 9,4:15pm,4:18pm,4:26pm,4:32pm,4:43pm,4:50pm,Departure 10,5:15pm,5:18pm,5:26pm,5:32pm,5:43pm,5:50pm,Departure 11,6:15pm,6:18pm,6:26pm,6:32pm,6:43pm,6:50pm,Departure 12,7:15pm,7:18pm,7:26pm,7:32pm,7:43pm,7:50pm,Departure 13,8:15pm,8:18pm,8:26pm,8:32pm,8:43pm,8:50pm,Departure 14,9:15pm,9:18pm,9:26pm,9:32pm,9:43pm,9:50pm,Departure 15,10:15pm,10:18pm,10:26pm,10:32pm,10:43pm,10:50pm,Departure 16,11:15pm,11:18pm,11:26pm,11:32pm,11:43pm,11:50pm,;Departure 1,9:00am,9:03am,9:11am,9:17am,9:28am,9:35am,Departure 2,10:00am,10:03am,10:11am,10:17am,10:28am,10:35am,Departure 3,11:00am,11:03am,11:11am,11:17am,11:28am,11:35am,Departure 4,12:00pm,12:03pm,12:11pm,12:17pm,12:28pm,12:35pm,Departure 5,1:00pm,1:03pm,1:11pm,1:17pm,1:28pm,1:35pm,Departure 6,2:00pm,2:03pm,2:11pm,2:17pm,2:28pm,2:35pm,Departure 7,3:00pm,3:03pm,3:11pm,3:17pm,3:28pm,3:35pm,Departure 8,4:00pm,4:03pm,4:11pm,4:17pm,4:28pm,4:35pm,Departure 9,5:00pm,5:03pm,5:11pm,5:17pm,5:28pm,5:35pm,Departure 10,6:00pm,6:03pm,6:11pm,6:17pm,6:28pm,6:35pm,Departure 11,7:00pm,7:03pm,7:11pm,7:17pm,7:28pm,7:35pm,;Forth St Leith Bridge;216 Highgate;Mornington Mailer St;168 Hillside Rd;271 Andersons Bay Rd;Departure 1,6:00am,6:16am,6:21am,6:28am,6:33am,Departure 2,6:30am,6:46am,6:51am,6:58am,7:03am,Departure 3,7:00am,7:16am,7:21am,7:28am,7:33am,Departure 4,7:30am,7:46am,7:52am,8:01am,8:05am,Departure 5,8:00am,8:16am,8:22am,8:31am,8:35am,Departure 6,8:30am,8:46am,8:51am,8:58am,9:03am,Departure 7,9:00am,9:16am,9:21am,9:28am,9:33am,Departure 8,9:30am,9:46am,9:51am,9:58am,10:03am,Departure 9,10:00am,10:16am,10:21am,10:28am,10:33am,Departure 10,10:30am,10:46am,10:51am,10:58am,11:03am,Departure 11,11:00am,11:16am,11:21am,11:28am,11:33am,Departure 12,11:30am,11:46am,11:51am,11:58am,12:03pm,Departure 13,12:00pm,12:16pm,12:21pm,12:28pm,12:33pm,Departure 14,12:30pm,12:46pm,12:51pm,12:58pm,1:03pm,Departure 15,1:00pm,1:16pm,1:21pm,1:28pm,1:33pm,Departure 16,1:30pm,1:46pm,1:51pm,1:58pm,2:03pm,Departure 17,2:00pm,2:16pm,2:21pm,2:28pm,2:33pm,Departure 18,2:30pm,2:46pm,2:51pm,2:58pm,3:03pm,Departure 19,3:00pm,3:16pm,3:21pm,3:28pm,3:33pm,Departure 20,3:30pm,3:46pm,3:51pm,3:58pm,4:03pm,Departure 21,4:00pm,4:16pm,4:21pm,4:28pm,4:33pm,Departure 22,4:30pm,4:46pm,4:51pm,4:58pm,5:03pm,Departure 23,5:00pm,5:16pm,5:22pm,5:31pm,5:35pm,Departure 24,5:30pm,5:46pm,5:52pm,6:01pm,6:05pm,Departure 25,6:00pm,6:16pm,6:21pm,6:28pm,6:33pm,Departure 26,6:30pm,6:46pm,6:51pm,6:58pm,7:03pm,Departure 27,7:30pm,7:46pm,7:51pm,7:58pm,8:03pm,Departure 28,8:30pm,8:46pm,8:51pm,8:58pm,9:03pm,Departure 29,9:30pm,9:46pm,9:51pm,9:58pm,10:03pm,Departure 30,10:30pm,10:46pm,10:51pm,10:58pm,11:03pm;Departure 1,8:15am,8:31am,8:37am,8:46am,8:50am,Departure 2,9:15am,9:31am,9:37am,9:46am,9:50am,Departure 3,10:15am,10:31am,10:37am,10:46am,10:50am,Departure 4,11:15am,11:31am,11:37am,11:46am,11:50am,Departure 5,12:15pm,12:31pm,12:37pm,12:46pm,12:50pm,Departure 6,1:15pm,1:31pm,1:37pm,1:46pm,1:50pm,Departure 7,2:15pm,2:31pm,2:37pm,2:46pm,2:50pm,Departure 8,3:15pm,3:31pm,3:37pm,3:46pm,3:50pm,Departure 9,4:15pm,4:31pm,4:37pm,4:46pm,4:50pm,Departure 10,5:15pm,5:31pm,5:37pm,5:46pm,5:50pm,Departure 11,6:15pm,6:31pm,6:37pm,6:46pm,6:50pm,Departure 12,7:15pm,7:31pm,7:37pm,7:46pm,7:50pm,Departure 13,8:15pm,8:31pm,8:37pm,8:46pm,8:50pm,Departure 14,9:15pm,9:31pm,9:37pm,9:46pm,9:50pm,Departure 15,10:15pm,10:31pm,10:37pm,10:46pm,10:50pm,Departure 16,11:15pm,11:31pm,11:37pm,11:46pm,11:50pm;Departure 1,9:00am,9:16am,9:22am,9:31am,9:35am,Departure 2,10:00am,10:16am,10:22am,10:31am,10:35am,Departure 3,11:00am,11:16am,11:22am,11:31am,11:35am,Departure 4,12:00pm,12:16pm,12:22pm,12:31pm,12:35pm,Departure 5,1:00pm,1:16pm,1:22pm,1:31pm,1:35pm,Departure 6,2:00pm,2:16pm,2:22pm,2:31pm,2:35pm,Departure 7,3:00pm,3:16pm,3:22pm,3:31pm,3:35pm,Departure 8,4:00pm,4:16pm,4:22pm,4:31pm,4:35pm,Departure 9,5:00pm,5:16pm,5:22pm,5:31pm,5:35pm,Departure 10,6:00pm,6:16pm,6:22pm,6:31pm,6:35pm,Departure 11,7:00pm,7:16pm,7:22pm,7:31pm,7:35pm;Harrington St, cnr Fox St;SH88, St Leonards Dr Nth;Bus Hub Stop G;Departure 1,6:10a.m.,6:23a.m.,6:41a.m.,Departure 2,6:40a.m.,6:53a.m.,7:11a.m.,Departure 3,7:10a.m.,7:23a.m.,7:41a.m.,Departure 4,7:30a.m.,7:43a.m.,8:01a.m.,Departure 5,7:50a.m.,8:03a.m.,8:21a.m.,Departure 6,8:10a.m.,8:23a.m.,8:41a.m.,Departure 7,8:40a.m.,8:53a.m.,9:11a.m.,Departure 8,9:10a.m.,9:23a.m.,9:41a.m.,Departure 9,9:40a.m.,9:53a.m.,10:11a.m.,Departure 10,10:10a.m.,10:23a.m.,10:41a.m.,Departure 11,10:40a.m.,10:53a.m.,11:11a.m.,Departure 12,11:10a.m.,11:23a.m.,11:41a.m.,Departure 13,11:40a.m.,11:53a.m.,12:11p.m.,Departure 14,12:10p.m.,12:23p.m.,12:41p.m.,Departure 15,12:40p.m.,12:53p.m.,1:11p.m.,Departure 16,1:10p.m.,1:23p.m.,1:41p.m.,Departure 17,1:40p.m.,1:53p.m.,2:11p.m.,Departure 18,2:10p.m.,2:23p.m.,2:41p.m.,Departure 19,2:40p.m.,2:53p.m.,3:11p.m.,Departure 20,3:10p.m.,3:23p.m.,3:41p.m.,Departure 21,3:40p.m.,3:53p.m.,4:11p.m.,Departure 22,4:10p.m.,4:23p.m.,4:41p.m.,Departure 23,4:40p.m.,4:53p.m.,5:11p.m.,Departure 24,5:10p.m.,5:23p.m.,5:41p.m.,Departure 25,5:40p.m.,5:53p.m.,6:11p.m.,Departure 26,6:10p.m.,6:23p.m.,6:41p.m.,Departure 27,6:40p.m.,6:53p.m.,7:11p.m.,Departure 28,7:10p.m.,7:23p.m.,7:41p.m.,Departure 29,8:10p.m.,8:23p.m.,8:41p.m.,Departure 30,9:10p.m.,9:23p.m.,9:41p.m.;Departure 1,6:10a.m.,6:23a.m.,6:41a.m.,Departure 2,6:40a.m.,6:53a.m.,7:11a.m.,Departure 3,7:10a.m.,7:23a.m.,7:41a.m.,Departure 4,7:30a.m.,7:43a.m.,8:01a.m.,Departure 5,7:50a.m.,8:03a.m.,8:21a.m.,Departure 6,8:10a.m.,8:23a.m.,8:41a.m.,Departure 7,8:40a.m.,8:53a.m.,9:11a.m.,Departure 8,9:10a.m.,9:23a.m.,9:41a.m.,Departure 9,9:40a.m.,9:53a.m.,10:11a.m.,Departure 10,10:10a.m.,10:23a.m.,10:41a.m.,Departure 11,10:40a.m.,10:53a.m.,11:11a.m.,Departure 12,11:10a.m.,11:23a.m.,11:41a.m.,Departure 13,11:40a.m.,11:53a.m.,12:11p.m.,Departure 14,12:10p.m.,12:23p.m.,12:41p.m.,Departure 15,12:40p.m.,12:53p.m.,1:11p.m.,Departure 16,1:10p.m.,1:23p.m.,1:41p.m.,Departure 17,1:40p.m.,1:53p.m.,2:11p.m.,Departure 18,2:10p.m.,2:23p.m.,2:41p.m.,Departure 19,2:40p.m.,2:53p.m.,3:11p.m.,Departure 20,3:10p.m.,3:23p.m.,3:41p.m.,Departure 21,3:40p.m.,3:53p.m.,4:11p.m.,Departure 22,4:10p.m.,4:23p.m.,4:41p.m.,Departure 23,4:40p.m.,4:53p.m.,5:11p.m.,Departure 24,5:10p.m.,5:23p.m.,5:41p.m.,Departure 25,5:40p.m.,5:53p.m.,6:11p.m.,Departure 26,6:10p.m.,6:23p.m.,6:41p.m.,Departure 27,6:40p.m.,6:53p.m.,7:11p.m.,Departure 28,7:10p.m.,7:23p.m.,7:41p.m.,Departure 29,8:10p.m.,8:23p.m.,8:41p.m.,Departure 30,9:10p.m.,9:23p.m.,9:41p.m.,Departure 31,10:10p.m.,10:23p.m.,10:41p.m.,Departure 32,11:10p.m.,11:23p.m.,11:41p.m.;Departure 1,8:10a.m.,8:23a.m.,8:41a.m.,Departure 2,9:10a.m.,9:23a.m.,9:41a.m.,Departure 3,10:10a.m.,10:23a.m.,10:41a.m.,Departure 4,11:10a.m.,11:23a.m.,11:41a.m.,Departure 5,12:10p.m.,12:23p.m.,12:41p.m.,Departure 6,1:10p.m.,1:23p.m.,1:41p.m.,Departure 7,2:10p.m.,2:23p.m.,2:41p.m.,Departure 8,3:10p.m.,3:23p.m.,3:41p.m.,Departure 9,4:10p.m.,4:23p.m.,4:41p.m.,Departure 10,5:10p.m.,5:23p.m.,5:41p.m.,Departure 11,6:10p.m.,6:23p.m.,6:41p.m.,Departure 12,7:10p.m.,7:23p.m.,7:41p.m.,Departure 13,8:10p.m.,8:23p.m.,8:41p.m.,Departure 14,9:10p.m.,9:23p.m.,9:41p.m.,Departure 15,10:10p.m.,10:23p.m.,10:41p.m.,Departure 16,11:10p.m.,11:23p.m.,11:41p.m.;Departure 1,8:10a.m.,8:23a.m.,8:41a.m.,Departure 2,9:10a.m.,9:23a.m.,9:41a.m.,Departure 3,10:10a.m.,10:23a.m.,10:41a.m.,Departure 4,11:10a.m.,11:23a.m.,11:41a.m.,Departure 5,12:10p.m.,12:23p.m.,12:41p.m.,Departure 6,1:10p.m.,1:23p.m.,1:41p.m.,Departure 7,2:10p.m.,2:23p.m.,2:41p.m.,Departure 8,3:10p.m.,3:23p.m.,3:41p.m.,Departure 9,4:10p.m.,4:23p.m.,4:41p.m.,Departure 10,5:10p.m.,5:23p.m.,5:41p.m.,Departure 11,6:10p.m.,6:23p.m.,6:41p.m.;Bus Hub Stop BSH88, St Leonards Dr NthCareys Bay HotelHarrington St, cnr Fox St;Departure 1,6:31a.m.,6:47a.m.,7:01a.m.,7:05a.m.,Departure 2,7:01a.m.,7:17a.m.,7:31a.m.,7:35a.m.,Departure 3,7:31a.m.,7:47a.m.,8:01a.m.,8:05a.m.,Departure 4,8:01a.m.,8:17a.m.,8:31a.m.,8:35a.m.,Departure 5,8:31a.m.,8:47a.m.,9:01a.m.,9:05a.m.,Departure 6,9:01a.m.,9:17a.m.,9:31a.m.,9:35a.m.,Departure 7,9:31a.m.,9:47a.m.,10:01a.m.,10:05a.m.,Departure 8,10:01a.m.,10:17a.m.,10:31a.m.,10:35a.m.,Departure 9,10:31a.m.,10:47a.m.,11:01a.m.,11:05a.m.,Departure 10,11:01a.m.,11:17a.m.,11:31a.m.,11:35a.m.,Departure 11,11:31a.m.,11:47a.m.,12:01p.m.,12:05p.m.,Departure 12,12:01p.m.,12:17p.m.,12:31p.m.,12:35p.m.,Departure 13,12:31p.m.,12:47p.m.,1:01p.m.,1:05p.m.,Departure 14,1:01p.m.,1:17p.m.,1:31p.m.,1:35p.m.,Departure 15,1:31p.m.,1:47p.m.,2:01p.m.,2:05p.m.,Departure 16,2:01p.m.,2:17p.m.,2:31p.m.,2:35p.m.,Departure 17,2:31p.m.,2:47p.m.,3:01p.m.,3:05p.m.,Departure 18,3:01p.m.,3:17p.m.,3:31p.m.,3:35p.m.,Departure 19,3:31p.m.,3:47p.m.,4:01p.m.,4:05p.m.,Departure 20,4:01p.m.,4:17p.m.,4:31p.m.,4:35p.m.,Departure 21,4:31p.m.,4:47p.m.,5:01p.m.,5:05p.m.,Departure 22,5:01p.m.,5:17p.m.,5:31p.m.,5:35p.m.,Departure 23,5:31p.m.,5:47p.m.,6:01p.m.,6:05p.m.,Departure 24,6:01p.m.,6:17p.m.,6:31p.m.,6:35p.m.,Departure 25,6:31p.m.,6:47p.m.,7:01p.m.,7:05p.m.,Departure 26,7:01p.m.,7:17p.m.,7:31p.m.,7:35p.m.,Departure 27,7:31p.m.,7:47p.m.,8:01p.m.,8:05p.m.,Departure 28,8:31p.m.,8:47p.m.,9:01p.m.,9:05p.m.,Departure 29,9:31p.m.,9:47p.m.,10:01p.m.,10:05p.m.;Departure 1,6:31a.m.,6:47a.m.,7:01a.m.,7:05a.m.,Departure 2,7:01a.m.,7:17a.m.,7:31a.m.,7:35a.m.,Departure 3,7:31a.m.,7:47a.m.,8:01a.m.,8:05a.m.,Departure 4,8:01a.m.,8:17a.m.,8:31a.m.,8:35a.m.,Departure 5,8:31a.m.,8:47a.m.,9:01a.m.,9:05a.m.,Departure 6,9:01a.m.,9:17a.m.,9:31a.m.,9:35a.m.,Departure 7,9:31a.m.,9:47a.m.,10:01a.m.,10:05a.m.,Departure 8,10:01a.m.,10:17a.m.,10:31a.m.,10:35a.m.,Departure 9,10:31a.m.,10:47a.m.,11:01a.m.,11:05a.m.,Departure 10,11:01a.m.,11:17a.m.,11:31a.m.,11:35a.m.,Departure 11,11:31a.m.,11:47a.m.,12:01p.m.,12:05p.m.,Departure 12,12:01p.m.,12:17p.m.,12:31p.m.,12:35p.m.,Departure 13,12:31p.m.,12:47p.m.,1:01p.m.,1:05p.m.,Departure 14,1:01p.m.,1:17p.m.,1:31p.m.,1:35p.m.,Departure 15,1:31p.m.,1:47p.m.,2:01p.m.,2:05p.m.,Departure 16,2:01p.m.,2:17p.m.,2:31p.m.,2:35p.m.,Departure 17,2:31p.m.,2:47p.m.,3:01p.m.,3:05p.m.,Departure 18,3:01p.m.,3:17p.m.,3:31p.m.,3:35p.m.,Departure 19,3:31p.m.,3:47p.m.,4:01p.m.,4:05p.m.,Departure 20,4:01p.m.,4:17p.m.,4:31p.m.,4:35p.m.,Departure 21,4:31p.m.,4:47p.m.,5:01p.m.,5:05p.m.,Departure 22,5:01p.m.,5:17p.m.,5:31p.m.,5:35p.m.,Departure 23,5:31p.m.,5:47p.m.,6:01p.m.,6:05p.m.,Departure 24,6:01p.m.,6:17p.m.,6:31p.m.,6:35p.m.,Departure 25,6:31p.m.,6:47p.m.,7:01p.m.,7:05p.m.,Departure 26,7:01p.m.,7:17p.m.,7:31p.m.,7:35p.m.,Departure 27,7:31p.m.,7:47p.m.,8:01p.m.,8:05p.m.,Departure 28,8:31p.m.,8:47p.m.,9:01p.m.,9:05p.m.,Departure 29,9:31p.m.,9:47p.m.,10:01p.m.,10:05p.m.,Departure 30,10:31p.m.,10:47p.m.,11:01p.m.,11:05p.m.,Departure 31,11:31p.m,11:47p.m.,12:01a.m.,12:05a.m.;Departure 1,8:31a.m.,8:47a.m.,9:01a.m.,9:05a.m.,Departure 2,9:31a.m.,9:47a.m.,10:01a.m.,10:05a.m.,Departure 3,10:31a.m.,10:47a.m.,11:01a.m.,11:05a.m.,Departure 4,11:31a.m.,11:47a.m.,12:01p.m.,12:05p.m.,Departure 5,12:31p.m.,12:47p.m.,1:01p.m.,1:05p.m.,Departure 6,1:31p.m.,1:47p.m.,2:01p.m.,2:05p.m.,Departure 7,2:31p.m.,2:47p.m.,3:01p.m.,3:05p.m.,Departure 8,3:31p.m.,3:47p.m.,4:01p.m.,4:05p.m.,Departure 9,4:31p.m.,4:47p.m.,5:01p.m.,5:05p.m.,Departure 10,5:31p.m.,5:47p.m.,6:01p.m.,6:05p.m.,Departure 11,6:31p.m.,6:47p.m.,7:01p.m.,7:05p.m.,Departure 12,7:31p.m.,7:47p.m.,8:01p.m.,8:05p.m.,Departure 13,8:31p.m.,8:47p.m.,9:01p.m.,9:05p.m.,Departure 14,9:31p.m.,9:47p.m.,10:01p.m.,10:05p.m.,Departure 15,10:31p.m.,10:47p.m.,11:01p.m.,11:05p.m.,Departure 16,11:31p.m.,11:47p.m.,12:01a.m.,12:05a.m.;Departure 1,8:31a.m.,8:47a.m.,9:01a.m.,9:05a.m.,Departure 2,9:31a.m.,9:47a.m.,10:01a.m.,10:05a.m.,Departure 3,10:31a.m.,10:47a.m.,11:01a.m.,11:05a.m.,Departure 4,11:31a.m.,11:47a.m.,12:01p.m.,12:05p.m.,Departure 5,12:31p.m.,12:47p.m.,1:01p.m.,1:05p.m.,Departure 6,1:31p.m.,1:47p.m.,2:01p.m.,2:05p.m.,Departure 7,2:31p.m.,2:47p.m.,3:01p.m.,3:05p.m.,Departure 8,3:31p.m.,3:47p.m.,4:01p.m.,4:05p.m.,Departure 9,4:31p.m.,4:47p.m.,5:01p.m.,5:05p.m.,Departure 10,5:31p.m.,5:47p.m.,6:01p.m.,6:05p.m.;2 Harington Pt Rd;Company Bay;Broad Bay;Macandrew Bay;Bus Hub Stop G;Departure 1,6:57am,7:04am,7:10am,7:13am,7:37am,Departure 2,7:27am,7:34am,7:40am,7:43am,8:07am,Departure 3,7:47am,7:54am,8:00am,8:03am,8:37am,Departure 4,8:27am,8:34am,8:40am,8:43am,9:07am,Departure 5,8:57am,9:04am,9:10am,9:13am,9:37am,Departure 6,9:59am,10:05am,10:10am,10:13am,10:34am,Departure 7,10:59am,11:05am,11:10am,11:13am,11:34am,Departure 8,11:59am,12:05pm,12:10pm,12:13pm,12:34pm,Departure 9,12:59pm,1:05pm,1:10pm,1:13pm,1:34pm,Departure 10,1:59pm,2:05pm,2:10pm,2:13pm,2:34pm,Departure 11,2:59pm,3:05pm,3:10pm,3:13pm,3:34pm,Departure 12,3:59pm,4:06pm,4:12pm,4:15pm,4:39pm,Departure 13,4:27pm,4:34pm,4:40pm,4:43pm,5:07pm,Departure 14,4:57pm,5:04pm,5:10pm,5:13pm,5:37pm,Departure 15,5:27pm,5:34pm,5:40pm,5:43pm,6:07pm,Departure 16,5:57pm,6:04pm,6:10pm,6:13pm,6:37pm,Departure 17,6:59pm,7:05pm,7:10pm,7:13pm,7:34pm,Departure 18,7:20pm,7:26pm,7:31pm,7:34pm,7:55pm,Departure 19,8:20pm,8:26pm,8:31pm,8:34pm,8:55pm,Departure 20,9:20pm,9:26pm,9:31pm,9:34pm,9:55pm;Departure 1,6:57am,7:04am,7:10am,7:13am,7:37am,Departure 2,7:27am,7:34am,7:40am,7:43am,8:07am,Departure 3,7:47am,7:54am,8:00am,8:03am,8:37am,Departure 4,8:27am,8:34am,8:40am,8:43am,9:07am,Departure 5,8:57am,9:04am,9:10am,9:13am,9:37am,Departure 6,9:59am,10:05am,10:10am,10:13am,10:34am,Departure 7,10:59am,11:05am,11:10am,11:13am,11:34am,Departure 8,11:59am,12:05pm,12:10pm,12:13pm,12:34pm,Departure 9,12:59pm,1:05pm,1:10pm,1:13pm,1:34pm,Departure 10,1:59pm,2:05pm,2:10pm,2:13pm,2:34pm,Departure 11,2:59pm,3:05pm,3:10pm,3:13pm,3:34pm,Departure 12,3:59pm,4:06pm,4:12pm,4:15pm,4:39pm,Departure 13,4:27pm,4:34pm,4:40pm,4:43pm,5:07pm,Departure 14,4:57pm,5:04pm,5:10pm,5:13pm,5:37pm,Departure 15,5:27pm,5:34pm,5:40pm,5:43pm,6:07pm,Departure 16,5:57pm,6:04pm,6:10pm,6:13pm,6:37pm,Departure 17,6:59pm,7:05pm,7:10pm,7:13pm,7:34pm,Departure 18,7:20pm,7:26pm,7:31pm,7:34pm,7:55pm,Departure 19,8:20pm,8:26pm,8:31pm,8:34pm,8:55pm,Departure 20,9:20pm,9:26pm,9:31pm,9:34pm,9:55pm,Departure 21,10:20pm,10:26pm,10:31pm,10:34pm,10:55pm,Departure 22,11:20pm,11:26pm,11:31pm,11:34pm,11:55pm;Departure 1,7:59am,8:05am,8:10am,8:13am,8:34am,Departure 2,8:59am,9:05am,9:10am,9:13am,9:34am,Departure 3,9:59am,10:05am,10:10am,10:13am,10:34am,Departure 4,10:59am,11:05am,11:10am,11:13am,11:34am,Departure 5,11:59am,12:05pm,12:10pm,12:13pm,12:34pm,Departure 6,12:59pm,1:05pm,1:10pm,1:13pm,1:34pm,Departure 7,1:59pm,2:05pm,2:10pm,2:13pm,2:34pm,Departure 8,2:59pm,3:05pm,3:10pm,3:13pm,3:34pm,Departure 9,3:59pm,4:05pm,4:10pm,4:13pm,4:34pm,Departure 10,4:59pm,5:05pm,5:10pm,5:13pm,5:34pm,Departure 11,5:59pm,6:05pm,6:10pm,6:13pm,6:34pm,Departure 12,6:59pm,7:05pm,7:10pm,7:13pm,7:34pm,Departure 13,7:20pm,7:26pm,7:31pm,7:34pm,7:55pm,Departure 14,8:20pm,8:26pm,8:31pm,8:34pm,8:55pm,Departure 15,9:20pm,9:26pm,9:31pm,9:34pm,9:55pm,Departure 16,10:20pm,10:26pm,10:31pm,10:34pm,10:55pm,Departure 17,11:20pm,11:26pm,11:31pm,11:34pm,11:55pm;Departure 1,7:59am,8:05am,8:10am,8:13am,8:34am,Departure 2,8:59am,9:05am,9:10am,9:13am,9:34am,Departure 3,9:59am,10:05am,10:10am,10:13am,10:34am,Departure 4,10:59am,11:05am,11:10am,11:13am,11:34am,Departure 5,11:59am,12:05pm,12:10pm,12:13pm,12:34pm,Departure 6,12:59pm,1:05pm,1:10pm,1:13pm,1:34pm,Departure 7,1:59pm,2:05pm,2:10pm,2:13pm,2:34pm,Departure 8,2:59pm,3:05pm,3:10pm,3:13pm,3:34pm,Departure 9,3:59pm,4:05pm,4:10pm,4:13pm,4:34pm,Departure 10,4:59pm,5:05pm,5:10pm,5:13pm,5:34pm,Departure 11,5:59pm,6:05pm,6:10pm,6:13pm,6:34pm,Departure 12,6:59pm,7:05pm,7:10pm,7:13pm,7:34pm,Departure 13,7:20pm,7:26pm,7:31pm,7:34pm,7:55pm,Departure 14,8:20pm,8:26pm,8:31pm,8:34pm,8:55pm;Bus Hub Stop G;Macandrew Bay;723 Portobello Rd;Broad Bay;7 Harington Pt Rd;Departure 1,7:38am,8:05am,8:08am,8:14am,8:24am,Departure 2,8:08am,8:35am,8:38am,8:44am,8:54am,Departure 3,8:38am,9:01am,9:04am,9:10am,9:19am,Departure 4,9:08am,9:35am,9:38am,9:44am,9:54am,Departure 5,9:38am,10:01am,10:04am,10:10am,10:19am,Departure 6,10:38am,11:01am,11:04am,11:10am,11:19am,Departure 7,11:38am,12:01pm,12:04pm,12:10pm,12:19pm,Departure 8,12:38pm,1:01pm,1:04pm,1:10pm,1:19pm,Departure 9,1:38pm,2:01pm,2:04pm,2:10pm,2:19pm,Departure 10,2:38pm,3:01pm,3:04pm,3:10pm,3:19pm,Departure 11,3:08pm,3:44pm,3:47pm,3:53pm,4:04pm,Departure 12,3:38pm,4:05pm,4:08pm,4:14pm,4:24pm,Departure 13,4:08pm,4:35pm,4:38pm,4:44pm,4:54pm,Departure 14,4:38pm,5:05pm,5:08pm,5:14pm,5:24pm,Departure 15,5:08pm,5:35pm,5:38pm,5:44pm,5:54pm,Departure 16,5:38pm,6:01pm,6:04pm,6:10pm,6:19pm,Departure 17,6:38pm,7:01pm,7:04pm,7:10pm,7:19pm,Departure 18,7:38pm,8:01pm,8:04pm,8:10pm,8:19pm,Departure 19,8:38pm,9:01pm,9:04pm,9:10pm,9:19pm,Departure 20,9:38pm,10:01pm,10:04pm,10:10pm,10:19pm,Departure 21,10:38pm,11:01pm,11:04pm,11:10pm,11:19pm,Departure 22,11:38pm,12:01am,12:04am,12:10am,12:19am;Departure 1,8:38am,9:01am,9:04am,9:10am,9:19am,Departure 2,9:38am,10:01am,10:04am,10:10am,10:19am,Departure 3,10:38am,11:01am,11:04am,11:10am,11:19am,Departure 4,11:38am,12:01pm,12:04pm,12:10pm,12:19pm,Departure 5,12:38pm,1:01pm,1:04pm,1:10pm,1:19pm,Departure 6,1:38pm,2:01pm,2:04pm,2:10pm,2:19pm,Departure 7,2:38pm,3:01pm,3:04pm,3:10pm,3:19pm,Departure 8,3:38pm,4:01pm,4:04pm,4:10pm,4:19pm,Departure 9,4:38pm,5:01pm,5:04pm,5:10pm,5:19pm,Departure 10,5:38pm,6:01pm,6:04pm,6:10pm,6:19pm,Departure 11,6:38pm,7:01pm,7:04pm,7:10pm,7:19pm,Departure 12,7:38pm,8:01pm,8:04pm,8:10pm,8:19pm,Departure 13,8:38pm,9:01pm,9:04pm,9:10pm,9:19pm,Departure 14,9:38pm,10:01pm,10:04pm,10:10pm,10:19pm,Departure 15,10:38pm,11:01pm,11:04pm,11:10pm,11:19pm,Departure 16,11:38pm,12:01am,12:04am,12:10am,12:19am;Departure 1,8:38am,9:01am,9:04am,9:10am,9:19am,Departure 2,9:38am,10:01am,10:04am,10:10am,10:19am,Departure 3,10:38am,11:01am,11:04am,11:10am,11:19am,Departure 4,11:38am,12:01pm,12:04pm,12:10pm,12:19pm,Departure 5,12:38pm,1:01pm,1:04pm,1:10pm,1:19pm,Departure 6,1:38pm,2:01pm,2:04pm,2:10pm,2:19pm,Departure 7,2:38pm,3:01pm,3:04pm,3:10pm,3:19pm,Departure 8,3:38pm,4:01pm,4:04pm,4:10pm,4:19pm,Departure 9,4:38pm,5:01pm,5:04pm,5:10pm,5:19pm,Departure 10,5:38pm,6:01pm,6:04pm,6:10pm,6:19pm,Departure 11,6:38pm,7:01pm,7:04pm,7:10pm,7:19pm,Departure 12,7:38pm,8:01pm,8:04pm,8:10pm,8:19pm,Departure 13,8:38pm,9:01pm,9:04pm,9:10pm,9:19pm</v>
+        <v>271 Andersons Bay Rd;169 Hillside Rd;2 Mailer St;271 Highgate;Great King St North Botanic Gardens;Forth St Leith Bridge;Departure 1,5:50am,5:53am,6:01am,6:07am,6:18am,6:25am,Departure 2,6:10am,6:13am,6:21am,6:27am,6:38am,6:45am,Departure 3,6:40am,6:43am,6:51am,6:57am,7:08am,7:15am,Departure 4,7:10am,7:13am,7:21am,7:27am,7:38am,7:45am,Departure 5,7:40am,7:43am,7:53am,7:59am,8:12am,8:20am,Departure 6,8:10am,8:13am,8:23am,8:29am,8:42am,8:50am,Departure 7,8:40am,8:43am,8:51am,8:57am,9:08am,9:15am,Departure 8,9:10am,9:13am,9:21am,9:27am,9:38am,9:45am,Departure 9,9:40am,9:43am,9:51am,9:57am,10:08am,10:15am,Departure 10,10:10am,10:13am,10:21am,10:27am,10:38am,10:45am,Departure 11,10:40am,10:43am,10:51am,10:57am,11:08am,11:15am,Departure 12,11:10am,11:13am,11:21am,11:27am,11:38am,11:45am,Departure 13,11:40am,11:43am,11:51am,11:57am,12:08pm,12:15pm,Departure 14,12:10pm,12:13pm,12:21pm,12:27pm,12:38pm,12:45pm,Departure 15,12:40pm,12:43pm,12:51pm,12:57pm,1:08pm,1:15pm,Departure 16,1:10pm,1:13pm,1:21pm,1:27pm,1:38pm,1:45pm,Departure 17,1:40pm,1:43pm,1:51pm,1:57pm,2:08pm,2:15pm,Departure 18,2:10pm,2:13pm,2:21pm,2:27pm,2:38pm,2:45pm,Departure 19,2:40pm,2:43pm,2:51pm,2:57pm,3:08pm,3:15pm,Departure 20,3:10pm,3:13pm,3:21pm,3:27pm,3:38pm,3:45pm,Departure 21,3:40pm,3:43pm,3:51pm,3:57pm,4:08pm,4:15pm,Departure 22,4:10pm,4:13pm,4:21pm,4:27pm,4:38pm,4:45pm,Departure 23,4:40pm,4:43pm,4:51pm,4:57pm,5:08pm,5:15pm,Departure 24,5:10pm,5:13pm,5:23pm,5:29pm,5:42pm,5:50pm,Departure 25,5:40pm,5:43pm,5:53pm,5:59pm,6:12pm,6:20pm,Departure 26,6:10pm,6:13pm,6:21pm,6:27pm,6:38pm,6:45pm,Departure 27,6:40pm,6:43pm,6:51pm,6:57pm,7:08pm,7:15pm,Departure 28,7:30pm,7:33pm,7:41pm,7:47pm,7:58pm,8:05pm,Departure 29,8:30pm,8:33pm,8:41pm,8:47pm,8:58pm,9:05pm,Departure 30,9:30pm,9:33pm,9:41pm,9:47pm,9:58pm,10:05pm,Departure 31,10:30pm,10:33pm,10:41pm,10:47pm,10:58pm,11:05pm,;Departure 1,8:15am,8:18am,8:26am,8:32am,8:43am,8:50am,Departure 2,9:15am,9:18am,9:26am,9:32am,9:43am,9:50am,Departure 3,10:15am,10:18am,10:26am,10:32am,10:43am,10:50am,Departure 4,11:15am,11:18am,11:26am,11:32am,11:43am,11:50am,Departure 5,12:15pm,12:18pm,12:26pm,12:32pm,12:43pm,12:50pm,Departure 6,1:15pm,1:18pm,1:26pm,1:32pm,1:43pm,1:50pm,Departure 7,2:15pm,2:18pm,2:26pm,2:32pm,2:43pm,2:50pm,Departure 8,3:15pm,3:18pm,3:26pm,3:32pm,3:43pm,3:50pm,Departure 9,4:15pm,4:18pm,4:26pm,4:32pm,4:43pm,4:50pm,Departure 10,5:15pm,5:18pm,5:26pm,5:32pm,5:43pm,5:50pm,Departure 11,6:15pm,6:18pm,6:26pm,6:32pm,6:43pm,6:50pm,Departure 12,7:15pm,7:18pm,7:26pm,7:32pm,7:43pm,7:50pm,Departure 13,8:15pm,8:18pm,8:26pm,8:32pm,8:43pm,8:50pm,Departure 14,9:15pm,9:18pm,9:26pm,9:32pm,9:43pm,9:50pm,Departure 15,10:15pm,10:18pm,10:26pm,10:32pm,10:43pm,10:50pm,Departure 16,11:15pm,11:18pm,11:26pm,11:32pm,11:43pm,11:50pm,;Departure 1,9:00am,9:03am,9:11am,9:17am,9:28am,9:35am,Departure 2,10:00am,10:03am,10:11am,10:17am,10:28am,10:35am,Departure 3,11:00am,11:03am,11:11am,11:17am,11:28am,11:35am,Departure 4,12:00pm,12:03pm,12:11pm,12:17pm,12:28pm,12:35pm,Departure 5,1:00pm,1:03pm,1:11pm,1:17pm,1:28pm,1:35pm,Departure 6,2:00pm,2:03pm,2:11pm,2:17pm,2:28pm,2:35pm,Departure 7,3:00pm,3:03pm,3:11pm,3:17pm,3:28pm,3:35pm,Departure 8,4:00pm,4:03pm,4:11pm,4:17pm,4:28pm,4:35pm,Departure 9,5:00pm,5:03pm,5:11pm,5:17pm,5:28pm,5:35pm,Departure 10,6:00pm,6:03pm,6:11pm,6:17pm,6:28pm,6:35pm,Departure 11,7:00pm,7:03pm,7:11pm,7:17pm,7:28pm,7:35pm,;Forth St Leith Bridge;216 Highgate;Mornington Mailer St;168 Hillside Rd;271 Andersons Bay Rd;Departure 1,6:00am,6:16am,6:21am,6:28am,6:33am,Departure 2,6:30am,6:46am,6:51am,6:58am,7:03am,Departure 3,7:00am,7:16am,7:21am,7:28am,7:33am,Departure 4,7:30am,7:46am,7:52am,8:01am,8:05am,Departure 5,8:00am,8:16am,8:22am,8:31am,8:35am,Departure 6,8:30am,8:46am,8:51am,8:58am,9:03am,Departure 7,9:00am,9:16am,9:21am,9:28am,9:33am,Departure 8,9:30am,9:46am,9:51am,9:58am,10:03am,Departure 9,10:00am,10:16am,10:21am,10:28am,10:33am,Departure 10,10:30am,10:46am,10:51am,10:58am,11:03am,Departure 11,11:00am,11:16am,11:21am,11:28am,11:33am,Departure 12,11:30am,11:46am,11:51am,11:58am,12:03pm,Departure 13,12:00pm,12:16pm,12:21pm,12:28pm,12:33pm,Departure 14,12:30pm,12:46pm,12:51pm,12:58pm,1:03pm,Departure 15,1:00pm,1:16pm,1:21pm,1:28pm,1:33pm,Departure 16,1:30pm,1:46pm,1:51pm,1:58pm,2:03pm,Departure 17,2:00pm,2:16pm,2:21pm,2:28pm,2:33pm,Departure 18,2:30pm,2:46pm,2:51pm,2:58pm,3:03pm,Departure 19,3:00pm,3:16pm,3:21pm,3:28pm,3:33pm,Departure 20,3:30pm,3:46pm,3:51pm,3:58pm,4:03pm,Departure 21,4:00pm,4:16pm,4:21pm,4:28pm,4:33pm,Departure 22,4:30pm,4:46pm,4:51pm,4:58pm,5:03pm,Departure 23,5:00pm,5:16pm,5:22pm,5:31pm,5:35pm,Departure 24,5:30pm,5:46pm,5:52pm,6:01pm,6:05pm,Departure 25,6:00pm,6:16pm,6:21pm,6:28pm,6:33pm,Departure 26,6:30pm,6:46pm,6:51pm,6:58pm,7:03pm,Departure 27,7:30pm,7:46pm,7:51pm,7:58pm,8:03pm,Departure 28,8:30pm,8:46pm,8:51pm,8:58pm,9:03pm,Departure 29,9:30pm,9:46pm,9:51pm,9:58pm,10:03pm,Departure 30,10:30pm,10:46pm,10:51pm,10:58pm,11:03pm;Departure 1,8:15am,8:31am,8:37am,8:46am,8:50am,Departure 2,9:15am,9:31am,9:37am,9:46am,9:50am,Departure 3,10:15am,10:31am,10:37am,10:46am,10:50am,Departure 4,11:15am,11:31am,11:37am,11:46am,11:50am,Departure 5,12:15pm,12:31pm,12:37pm,12:46pm,12:50pm,Departure 6,1:15pm,1:31pm,1:37pm,1:46pm,1:50pm,Departure 7,2:15pm,2:31pm,2:37pm,2:46pm,2:50pm,Departure 8,3:15pm,3:31pm,3:37pm,3:46pm,3:50pm,Departure 9,4:15pm,4:31pm,4:37pm,4:46pm,4:50pm,Departure 10,5:15pm,5:31pm,5:37pm,5:46pm,5:50pm,Departure 11,6:15pm,6:31pm,6:37pm,6:46pm,6:50pm,Departure 12,7:15pm,7:31pm,7:37pm,7:46pm,7:50pm,Departure 13,8:15pm,8:31pm,8:37pm,8:46pm,8:50pm,Departure 14,9:15pm,9:31pm,9:37pm,9:46pm,9:50pm,Departure 15,10:15pm,10:31pm,10:37pm,10:46pm,10:50pm,Departure 16,11:15pm,11:31pm,11:37pm,11:46pm,11:50pm;Departure 1,9:00am,9:16am,9:22am,9:31am,9:35am,Departure 2,10:00am,10:16am,10:22am,10:31am,10:35am,Departure 3,11:00am,11:16am,11:22am,11:31am,11:35am,Departure 4,12:00pm,12:16pm,12:22pm,12:31pm,12:35pm,Departure 5,1:00pm,1:16pm,1:22pm,1:31pm,1:35pm,Departure 6,2:00pm,2:16pm,2:22pm,2:31pm,2:35pm,Departure 7,3:00pm,3:16pm,3:22pm,3:31pm,3:35pm,Departure 8,4:00pm,4:16pm,4:22pm,4:31pm,4:35pm,Departure 9,5:00pm,5:16pm,5:22pm,5:31pm,5:35pm,Departure 10,6:00pm,6:16pm,6:22pm,6:31pm,6:35pm,Departure 11,7:00pm,7:16pm,7:22pm,7:31pm,7:35pm;Harrington St, cnr Fox St;SH88, St Leonards Dr Nth;Bus Hub Stop G;Departure 1,6:10a.m.,6:23a.m.,6:41a.m.,Departure 2,6:40a.m.,6:53a.m.,7:11a.m.,Departure 3,7:10a.m.,7:23a.m.,7:41a.m.,Departure 4,7:30a.m.,7:43a.m.,8:01a.m.,Departure 5,7:50a.m.,8:03a.m.,8:21a.m.,Departure 6,8:10a.m.,8:23a.m.,8:41a.m.,Departure 7,8:40a.m.,8:53a.m.,9:11a.m.,Departure 8,9:10a.m.,9:23a.m.,9:41a.m.,Departure 9,9:40a.m.,9:53a.m.,10:11a.m.,Departure 10,10:10a.m.,10:23a.m.,10:41a.m.,Departure 11,10:40a.m.,10:53a.m.,11:11a.m.,Departure 12,11:10a.m.,11:23a.m.,11:41a.m.,Departure 13,11:40a.m.,11:53a.m.,12:11p.m.,Departure 14,12:10p.m.,12:23p.m.,12:41p.m.,Departure 15,12:40p.m.,12:53p.m.,1:11p.m.,Departure 16,1:10p.m.,1:23p.m.,1:41p.m.,Departure 17,1:40p.m.,1:53p.m.,2:11p.m.,Departure 18,2:10p.m.,2:23p.m.,2:41p.m.,Departure 19,2:40p.m.,2:53p.m.,3:11p.m.,Departure 20,3:10p.m.,3:23p.m.,3:41p.m.,Departure 21,3:40p.m.,3:53p.m.,4:11p.m.,Departure 22,4:10p.m.,4:23p.m.,4:41p.m.,Departure 23,4:40p.m.,4:53p.m.,5:11p.m.,Departure 24,5:10p.m.,5:23p.m.,5:41p.m.,Departure 25,5:40p.m.,5:53p.m.,6:11p.m.,Departure 26,6:10p.m.,6:23p.m.,6:41p.m.,Departure 27,6:40p.m.,6:53p.m.,7:11p.m.,Departure 28,7:10p.m.,7:23p.m.,7:41p.m.,Departure 29,8:10p.m.,8:23p.m.,8:41p.m.,Departure 30,9:10p.m.,9:23p.m.,9:41p.m.;Departure 1,6:10a.m.,6:23a.m.,6:41a.m.,Departure 2,6:40a.m.,6:53a.m.,7:11a.m.,Departure 3,7:10a.m.,7:23a.m.,7:41a.m.,Departure 4,7:30a.m.,7:43a.m.,8:01a.m.,Departure 5,7:50a.m.,8:03a.m.,8:21a.m.,Departure 6,8:10a.m.,8:23a.m.,8:41a.m.,Departure 7,8:40a.m.,8:53a.m.,9:11a.m.,Departure 8,9:10a.m.,9:23a.m.,9:41a.m.,Departure 9,9:40a.m.,9:53a.m.,10:11a.m.,Departure 10,10:10a.m.,10:23a.m.,10:41a.m.,Departure 11,10:40a.m.,10:53a.m.,11:11a.m.,Departure 12,11:10a.m.,11:23a.m.,11:41a.m.,Departure 13,11:40a.m.,11:53a.m.,12:11p.m.,Departure 14,12:10p.m.,12:23p.m.,12:41p.m.,Departure 15,12:40p.m.,12:53p.m.,1:11p.m.,Departure 16,1:10p.m.,1:23p.m.,1:41p.m.,Departure 17,1:40p.m.,1:53p.m.,2:11p.m.,Departure 18,2:10p.m.,2:23p.m.,2:41p.m.,Departure 19,2:40p.m.,2:53p.m.,3:11p.m.,Departure 20,3:10p.m.,3:23p.m.,3:41p.m.,Departure 21,3:40p.m.,3:53p.m.,4:11p.m.,Departure 22,4:10p.m.,4:23p.m.,4:41p.m.,Departure 23,4:40p.m.,4:53p.m.,5:11p.m.,Departure 24,5:10p.m.,5:23p.m.,5:41p.m.,Departure 25,5:40p.m.,5:53p.m.,6:11p.m.,Departure 26,6:10p.m.,6:23p.m.,6:41p.m.,Departure 27,6:40p.m.,6:53p.m.,7:11p.m.,Departure 28,7:10p.m.,7:23p.m.,7:41p.m.,Departure 29,8:10p.m.,8:23p.m.,8:41p.m.,Departure 30,9:10p.m.,9:23p.m.,9:41p.m.,Departure 31,10:10p.m.,10:23p.m.,10:41p.m.,Departure 32,11:10p.m.,11:23p.m.,11:41p.m.;Departure 1,8:10a.m.,8:23a.m.,8:41a.m.,Departure 2,9:10a.m.,9:23a.m.,9:41a.m.,Departure 3,10:10a.m.,10:23a.m.,10:41a.m.,Departure 4,11:10a.m.,11:23a.m.,11:41a.m.,Departure 5,12:10p.m.,12:23p.m.,12:41p.m.,Departure 6,1:10p.m.,1:23p.m.,1:41p.m.,Departure 7,2:10p.m.,2:23p.m.,2:41p.m.,Departure 8,3:10p.m.,3:23p.m.,3:41p.m.,Departure 9,4:10p.m.,4:23p.m.,4:41p.m.,Departure 10,5:10p.m.,5:23p.m.,5:41p.m.,Departure 11,6:10p.m.,6:23p.m.,6:41p.m.,Departure 12,7:10p.m.,7:23p.m.,7:41p.m.,Departure 13,8:10p.m.,8:23p.m.,8:41p.m.,Departure 14,9:10p.m.,9:23p.m.,9:41p.m.,Departure 15,10:10p.m.,10:23p.m.,10:41p.m.,Departure 16,11:10p.m.,11:23p.m.,11:41p.m.;Departure 1,8:10a.m.,8:23a.m.,8:41a.m.,Departure 2,9:10a.m.,9:23a.m.,9:41a.m.,Departure 3,10:10a.m.,10:23a.m.,10:41a.m.,Departure 4,11:10a.m.,11:23a.m.,11:41a.m.,Departure 5,12:10p.m.,12:23p.m.,12:41p.m.,Departure 6,1:10p.m.,1:23p.m.,1:41p.m.,Departure 7,2:10p.m.,2:23p.m.,2:41p.m.,Departure 8,3:10p.m.,3:23p.m.,3:41p.m.,Departure 9,4:10p.m.,4:23p.m.,4:41p.m.,Departure 10,5:10p.m.,5:23p.m.,5:41p.m.,Departure 11,6:10p.m.,6:23p.m.,6:41p.m.;Bus Hub Stop BSH88, St Leonards Dr NthCareys Bay HotelHarrington St, cnr Fox St;Departure 1,6:31a.m.,6:47a.m.,7:01a.m.,7:05a.m.,Departure 2,7:01a.m.,7:17a.m.,7:31a.m.,7:35a.m.,Departure 3,7:31a.m.,7:47a.m.,8:01a.m.,8:05a.m.,Departure 4,8:01a.m.,8:17a.m.,8:31a.m.,8:35a.m.,Departure 5,8:31a.m.,8:47a.m.,9:01a.m.,9:05a.m.,Departure 6,9:01a.m.,9:17a.m.,9:31a.m.,9:35a.m.,Departure 7,9:31a.m.,9:47a.m.,10:01a.m.,10:05a.m.,Departure 8,10:01a.m.,10:17a.m.,10:31a.m.,10:35a.m.,Departure 9,10:31a.m.,10:47a.m.,11:01a.m.,11:05a.m.,Departure 10,11:01a.m.,11:17a.m.,11:31a.m.,11:35a.m.,Departure 11,11:31a.m.,11:47a.m.,12:01p.m.,12:05p.m.,Departure 12,12:01p.m.,12:17p.m.,12:31p.m.,12:35p.m.,Departure 13,12:31p.m.,12:47p.m.,1:01p.m.,1:05p.m.,Departure 14,1:01p.m.,1:17p.m.,1:31p.m.,1:35p.m.,Departure 15,1:31p.m.,1:47p.m.,2:01p.m.,2:05p.m.,Departure 16,2:01p.m.,2:17p.m.,2:31p.m.,2:35p.m.,Departure 17,2:31p.m.,2:47p.m.,3:01p.m.,3:05p.m.,Departure 18,3:01p.m.,3:17p.m.,3:31p.m.,3:35p.m.,Departure 19,3:31p.m.,3:47p.m.,4:01p.m.,4:05p.m.,Departure 20,4:01p.m.,4:17p.m.,4:31p.m.,4:35p.m.,Departure 21,4:31p.m.,4:47p.m.,5:01p.m.,5:05p.m.,Departure 22,5:01p.m.,5:17p.m.,5:31p.m.,5:35p.m.,Departure 23,5:31p.m.,5:47p.m.,6:01p.m.,6:05p.m.,Departure 24,6:01p.m.,6:17p.m.,6:31p.m.,6:35p.m.,Departure 25,6:31p.m.,6:47p.m.,7:01p.m.,7:05p.m.,Departure 26,7:01p.m.,7:17p.m.,7:31p.m.,7:35p.m.,Departure 27,7:31p.m.,7:47p.m.,8:01p.m.,8:05p.m.,Departure 28,8:31p.m.,8:47p.m.,9:01p.m.,9:05p.m.,Departure 29,9:31p.m.,9:47p.m.,10:01p.m.,10:05p.m.;Departure 1,6:31a.m.,6:47a.m.,7:01a.m.,7:05a.m.,Departure 2,7:01a.m.,7:17a.m.,7:31a.m.,7:35a.m.,Departure 3,7:31a.m.,7:47a.m.,8:01a.m.,8:05a.m.,Departure 4,8:01a.m.,8:17a.m.,8:31a.m.,8:35a.m.,Departure 5,8:31a.m.,8:47a.m.,9:01a.m.,9:05a.m.,Departure 6,9:01a.m.,9:17a.m.,9:31a.m.,9:35a.m.,Departure 7,9:31a.m.,9:47a.m.,10:01a.m.,10:05a.m.,Departure 8,10:01a.m.,10:17a.m.,10:31a.m.,10:35a.m.,Departure 9,10:31a.m.,10:47a.m.,11:01a.m.,11:05a.m.,Departure 10,11:01a.m.,11:17a.m.,11:31a.m.,11:35a.m.,Departure 11,11:31a.m.,11:47a.m.,12:01p.m.,12:05p.m.,Departure 12,12:01p.m.,12:17p.m.,12:31p.m.,12:35p.m.,Departure 13,12:31p.m.,12:47p.m.,1:01p.m.,1:05p.m.,Departure 14,1:01p.m.,1:17p.m.,1:31p.m.,1:35p.m.,Departure 15,1:31p.m.,1:47p.m.,2:01p.m.,2:05p.m.,Departure 16,2:01p.m.,2:17p.m.,2:31p.m.,2:35p.m.,Departure 17,2:31p.m.,2:47p.m.,3:01p.m.,3:05p.m.,Departure 18,3:01p.m.,3:17p.m.,3:31p.m.,3:35p.m.,Departure 19,3:31p.m.,3:47p.m.,4:01p.m.,4:05p.m.,Departure 20,4:01p.m.,4:17p.m.,4:31p.m.,4:35p.m.,Departure 21,4:31p.m.,4:47p.m.,5:01p.m.,5:05p.m.,Departure 22,5:01p.m.,5:17p.m.,5:31p.m.,5:35p.m.,Departure 23,5:31p.m.,5:47p.m.,6:01p.m.,6:05p.m.,Departure 24,6:01p.m.,6:17p.m.,6:31p.m.,6:35p.m.,Departure 25,6:31p.m.,6:47p.m.,7:01p.m.,7:05p.m.,Departure 26,7:01p.m.,7:17p.m.,7:31p.m.,7:35p.m.,Departure 27,7:31p.m.,7:47p.m.,8:01p.m.,8:05p.m.,Departure 28,8:31p.m.,8:47p.m.,9:01p.m.,9:05p.m.,Departure 29,9:31p.m.,9:47p.m.,10:01p.m.,10:05p.m.,Departure 30,10:31p.m.,10:47p.m.,11:01p.m.,11:05p.m.,Departure 31,11:31p.m,11:47p.m.,12:01a.m.,12:05a.m.;Departure 1,8:31a.m.,8:47a.m.,9:01a.m.,9:05a.m.,Departure 2,9:31a.m.,9:47a.m.,10:01a.m.,10:05a.m.,Departure 3,10:31a.m.,10:47a.m.,11:01a.m.,11:05a.m.,Departure 4,11:31a.m.,11:47a.m.,12:01p.m.,12:05p.m.,Departure 5,12:31p.m.,12:47p.m.,1:01p.m.,1:05p.m.,Departure 6,1:31p.m.,1:47p.m.,2:01p.m.,2:05p.m.,Departure 7,2:31p.m.,2:47p.m.,3:01p.m.,3:05p.m.,Departure 8,3:31p.m.,3:47p.m.,4:01p.m.,4:05p.m.,Departure 9,4:31p.m.,4:47p.m.,5:01p.m.,5:05p.m.,Departure 10,5:31p.m.,5:47p.m.,6:01p.m.,6:05p.m.,Departure 11,6:31p.m.,6:47p.m.,7:01p.m.,7:05p.m.,Departure 12,7:31p.m.,7:47p.m.,8:01p.m.,8:05p.m.,Departure 13,8:31p.m.,8:47p.m.,9:01p.m.,9:05p.m.,Departure 14,9:31p.m.,9:47p.m.,10:01p.m.,10:05p.m.,Departure 15,10:31p.m.,10:47p.m.,11:01p.m.,11:05p.m.,Departure 16,11:31p.m.,11:47p.m.,12:01a.m.,12:05a.m.;Departure 1,8:31a.m.,8:47a.m.,9:01a.m.,9:05a.m.,Departure 2,9:31a.m.,9:47a.m.,10:01a.m.,10:05a.m.,Departure 3,10:31a.m.,10:47a.m.,11:01a.m.,11:05a.m.,Departure 4,11:31a.m.,11:47a.m.,12:01p.m.,12:05p.m.,Departure 5,12:31p.m.,12:47p.m.,1:01p.m.,1:05p.m.,Departure 6,1:31p.m.,1:47p.m.,2:01p.m.,2:05p.m.,Departure 7,2:31p.m.,2:47p.m.,3:01p.m.,3:05p.m.,Departure 8,3:31p.m.,3:47p.m.,4:01p.m.,4:05p.m.,Departure 9,4:31p.m.,4:47p.m.,5:01p.m.,5:05p.m.,Departure 10,5:31p.m.,5:47p.m.,6:01p.m.,6:05p.m.;2 Harington Pt Rd;Company Bay;Broad Bay;Macandrew Bay;Bus Hub Stop G;Departure 1,6:57am,7:04am,7:10am,7:13am,7:37am,Departure 2,7:27am,7:34am,7:40am,7:43am,8:07am,Departure 3,7:47am,7:54am,8:00am,8:03am,8:37am,Departure 4,8:27am,8:34am,8:40am,8:43am,9:07am,Departure 5,8:57am,9:04am,9:10am,9:13am,9:37am,Departure 6,9:59am,10:05am,10:10am,10:13am,10:34am,Departure 7,10:59am,11:05am,11:10am,11:13am,11:34am,Departure 8,11:59am,12:05pm,12:10pm,12:13pm,12:34pm,Departure 9,12:59pm,1:05pm,1:10pm,1:13pm,1:34pm,Departure 10,1:59pm,2:05pm,2:10pm,2:13pm,2:34pm,Departure 11,2:59pm,3:05pm,3:10pm,3:13pm,3:34pm,Departure 12,3:59pm,4:06pm,4:12pm,4:15pm,4:39pm,Departure 13,4:27pm,4:34pm,4:40pm,4:43pm,5:07pm,Departure 14,4:57pm,5:04pm,5:10pm,5:13pm,5:37pm,Departure 15,5:27pm,5:34pm,5:40pm,5:43pm,6:07pm,Departure 16,5:57pm,6:04pm,6:10pm,6:13pm,6:37pm,Departure 17,6:59pm,7:05pm,7:10pm,7:13pm,7:34pm,Departure 18,7:20pm,7:26pm,7:31pm,7:34pm,7:55pm,Departure 19,8:20pm,8:26pm,8:31pm,8:34pm,8:55pm,Departure 20,9:20pm,9:26pm,9:31pm,9:34pm,9:55pm;Departure 1,6:57am,7:04am,7:10am,7:13am,7:37am,Departure 2,7:27am,7:34am,7:40am,7:43am,8:07am,Departure 3,7:47am,7:54am,8:00am,8:03am,8:37am,Departure 4,8:27am,8:34am,8:40am,8:43am,9:07am,Departure 5,8:57am,9:04am,9:10am,9:13am,9:37am,Departure 6,9:59am,10:05am,10:10am,10:13am,10:34am,Departure 7,10:59am,11:05am,11:10am,11:13am,11:34am,Departure 8,11:59am,12:05pm,12:10pm,12:13pm,12:34pm,Departure 9,12:59pm,1:05pm,1:10pm,1:13pm,1:34pm,Departure 10,1:59pm,2:05pm,2:10pm,2:13pm,2:34pm,Departure 11,2:59pm,3:05pm,3:10pm,3:13pm,3:34pm,Departure 12,3:59pm,4:06pm,4:12pm,4:15pm,4:39pm,Departure 13,4:27pm,4:34pm,4:40pm,4:43pm,5:07pm,Departure 14,4:57pm,5:04pm,5:10pm,5:13pm,5:37pm,Departure 15,5:27pm,5:34pm,5:40pm,5:43pm,6:07pm,Departure 16,5:57pm,6:04pm,6:10pm,6:13pm,6:37pm,Departure 17,6:59pm,7:05pm,7:10pm,7:13pm,7:34pm,Departure 18,7:20pm,7:26pm,7:31pm,7:34pm,7:55pm,Departure 19,8:20pm,8:26pm,8:31pm,8:34pm,8:55pm,Departure 20,9:20pm,9:26pm,9:31pm,9:34pm,9:55pm,Departure 21,10:20pm,10:26pm,10:31pm,10:34pm,10:55pm,Departure 22,11:20pm,11:26pm,11:31pm,11:34pm,11:55pm;Departure 1,7:59am,8:05am,8:10am,8:13am,8:34am,Departure 2,8:59am,9:05am,9:10am,9:13am,9:34am,Departure 3,9:59am,10:05am,10:10am,10:13am,10:34am,Departure 4,10:59am,11:05am,11:10am,11:13am,11:34am,Departure 5,11:59am,12:05pm,12:10pm,12:13pm,12:34pm,Departure 6,12:59pm,1:05pm,1:10pm,1:13pm,1:34pm,Departure 7,1:59pm,2:05pm,2:10pm,2:13pm,2:34pm,Departure 8,2:59pm,3:05pm,3:10pm,3:13pm,3:34pm,Departure 9,3:59pm,4:05pm,4:10pm,4:13pm,4:34pm,Departure 10,4:59pm,5:05pm,5:10pm,5:13pm,5:34pm,Departure 11,5:59pm,6:05pm,6:10pm,6:13pm,6:34pm,Departure 12,6:59pm,7:05pm,7:10pm,7:13pm,7:34pm,Departure 13,7:20pm,7:26pm,7:31pm,7:34pm,7:55pm,Departure 14,8:20pm,8:26pm,8:31pm,8:34pm,8:55pm,Departure 15,9:20pm,9:26pm,9:31pm,9:34pm,9:55pm,Departure 16,10:20pm,10:26pm,10:31pm,10:34pm,10:55pm,Departure 17,11:20pm,11:26pm,11:31pm,11:34pm,11:55pm;Departure 1,7:59am,8:05am,8:10am,8:13am,8:34am,Departure 2,8:59am,9:05am,9:10am,9:13am,9:34am,Departure 3,9:59am,10:05am,10:10am,10:13am,10:34am,Departure 4,10:59am,11:05am,11:10am,11:13am,11:34am,Departure 5,11:59am,12:05pm,12:10pm,12:13pm,12:34pm,Departure 6,12:59pm,1:05pm,1:10pm,1:13pm,1:34pm,Departure 7,1:59pm,2:05pm,2:10pm,2:13pm,2:34pm,Departure 8,2:59pm,3:05pm,3:10pm,3:13pm,3:34pm,Departure 9,3:59pm,4:05pm,4:10pm,4:13pm,4:34pm,Departure 10,4:59pm,5:05pm,5:10pm,5:13pm,5:34pm,Departure 11,5:59pm,6:05pm,6:10pm,6:13pm,6:34pm,Departure 12,6:59pm,7:05pm,7:10pm,7:13pm,7:34pm,Departure 13,7:20pm,7:26pm,7:31pm,7:34pm,7:55pm,Departure 14,8:20pm,8:26pm,8:31pm,8:34pm,8:55pm;Bus Hub Stop G;Macandrew Bay;723 Portobello Rd;Broad Bay;7 Harington Pt Rd;Departure 1,7:38am,8:05am,8:08am,8:14am,8:24am,Departure 2,8:08am,8:35am,8:38am,8:44am,8:54am,Departure 3,8:38am,9:01am,9:04am,9:10am,9:19am,Departure 4,9:08am,9:35am,9:38am,9:44am,9:54am,Departure 5,9:38am,10:01am,10:04am,10:10am,10:19am,Departure 6,10:38am,11:01am,11:04am,11:10am,11:19am,Departure 7,11:38am,12:01pm,12:04pm,12:10pm,12:19pm,Departure 8,12:38pm,1:01pm,1:04pm,1:10pm,1:19pm,Departure 9,1:38pm,2:01pm,2:04pm,2:10pm,2:19pm,Departure 10,2:38pm,3:01pm,3:04pm,3:10pm,3:19pm,Departure 11,3:08pm,3:44pm,3:47pm,3:53pm,4:04pm,Departure 12,3:38pm,4:05pm,4:08pm,4:14pm,4:24pm,Departure 13,4:08pm,4:35pm,4:38pm,4:44pm,4:54pm,Departure 14,4:38pm,5:05pm,5:08pm,5:14pm,5:24pm,Departure 15,5:08pm,5:35pm,5:38pm,5:44pm,5:54pm,Departure 16,5:38pm,6:01pm,6:04pm,6:10pm,6:19pm,Departure 17,6:38pm,7:01pm,7:04pm,7:10pm,7:19pm,Departure 18,7:38pm,8:01pm,8:04pm,8:10pm,8:19pm,Departure 19,8:38pm,9:01pm,9:04pm,9:10pm,9:19pm,Departure 20,9:38pm,10:01pm,10:04pm,10:10pm,10:19pm,Departure 21,10:38pm,11:01pm,11:04pm,11:10pm,11:19pm,Departure 22,11:38pm,12:01am,12:04am,12:10am,12:19am;Departure 1,8:38am,9:01am,9:04am,9:10am,9:19am,Departure 2,9:38am,10:01am,10:04am,10:10am,10:19am,Departure 3,10:38am,11:01am,11:04am,11:10am,11:19am,Departure 4,11:38am,12:01pm,12:04pm,12:10pm,12:19pm,Departure 5,12:38pm,1:01pm,1:04pm,1:10pm,1:19pm,Departure 6,1:38pm,2:01pm,2:04pm,2:10pm,2:19pm,Departure 7,2:38pm,3:01pm,3:04pm,3:10pm,3:19pm,Departure 8,3:38pm,4:01pm,4:04pm,4:10pm,4:19pm,Departure 9,4:38pm,5:01pm,5:04pm,5:10pm,5:19pm,Departure 10,5:38pm,6:01pm,6:04pm,6:10pm,6:19pm,Departure 11,6:38pm,7:01pm,7:04pm,7:10pm,7:19pm,Departure 12,7:38pm,8:01pm,8:04pm,8:10pm,8:19pm,Departure 13,8:38pm,9:01pm,9:04pm,9:10pm,9:19pm,Departure 14,9:38pm,10:01pm,10:04pm,10:10pm,10:19pm,Departure 15,10:38pm,11:01pm,11:04pm,11:10pm,11:19pm,Departure 16,11:38pm,12:01am,12:04am,12:10am,12:19am;Departure 1,8:38am,9:01am,9:04am,9:10am,9:19am,Departure 2,9:38am,10:01am,10:04am,10:10am,10:19am,Departure 3,10:38am,11:01am,11:04am,11:10am,11:19am,Departure 4,11:38am,12:01pm,12:04pm,12:10pm,12:19pm,Departure 5,12:38pm,1:01pm,1:04pm,1:10pm,1:19pm,Departure 6,1:38pm,2:01pm,2:04pm,2:10pm,2:19pm,Departure 7,2:38pm,3:01pm,3:04pm,3:10pm,3:19pm,Departure 8,3:38pm,4:01pm,4:04pm,4:10pm,4:19pm,Departure 9,4:38pm,5:01pm,5:04pm,5:10pm,5:19pm,Departure 10,5:38pm,6:01pm,6:04pm,6:10pm,6:19pm,Departure 11,6:38pm,7:01pm,7:04pm,7:10pm,7:19pm,Departure 12,7:38pm,8:01pm,8:04pm,8:10pm,8:19pm,Departure 13,8:38pm,9:01pm,9:04pm,9:10pm,9:19pm;Mosgiel Terminus;Fairfield, cnr Fairplay St;Green Is. (Inbound);Bus Hub Stop F;Departure 1,6:00am,6:15am,6:20am,6:37am,Departure 2,6:30am,6:45am,6:50am,7:07am,Departure 3,7:00am,7:15am,7:20am,7:37am,Departure 4,7:15am,7:30am,7:35am,7:52am,Departure 5,7:30am,7:45am,7:50am,8:07am,Departure 6,7:45am,8:00am,8:05am,8:22am,Departure 7,8:00am,8:15am,8:20am,8:37am,Departure 8,8:15am,8:30am,8:35am,8:52am,Departure 9,8:30am,8:45am,8:50am,9:07am,Departure 10,8:45am,9:00am,9:05am,9:22am,Departure 11,9:00am,9:15am,9:20am,9:37am,Departure 12,9:30am,9:45am,9:50am,10:07am,Departure 13,10:00am,10:15am,10:20am,10:37am,Departure 14,10:30am,10:45am,10:50am,11:07am,Departure 15,11:00am,11:15am,11:20am,11:37am,Departure 16,11:30am,11:45am,11:50am,12:07pm,Departure 17,12:00pm,12:15pm,12:20pm,12:37pm,Departure 18,12:30pm,12:45pm,12:50pm,1:07pm,Departure 19,1:00pm,1:15pm,1:20pm,1:37pm,Departure 20,1:30pm,1:45pm,1:50pm,2:07pm,Departure 21,2:00pm,2:15pm,2:20pm,2:37pm,Departure 22,2:30pm,2:45pm,2:50pm,3:07pm,Departure 23,3:00pm,3:15pm,3:20pm,3:37pm,Departure 24,3:15pm,3:30pm,3:35pm,3:52pm,Departure 25,3:30pm,3:45pm,3:50pm,4:07pm,Departure 26,3:45pm,4:00pm,4:05pm,4:22pm,Departure 27,4:00pm,4:15pm,4:20pm,4:37pm,Departure 28,4:15pm,4:30pm,4:35pm,4:52pm,Departure 29,4:30pm,4:45pm,4:50pm,5:07pm,Departure 30,4:45pm,5:00pm,5:05pm,5:22pm,Departure 31,5:00pm,5:15pm,5:20pm,5:37pm,Departure 32,5:30pm,5:45pm,5:50pm,6:07pm,Departure 33,6:00pm,6:15pm,6:20pm,6:37pm,Departure 34,6:30pm,6:45pm,6:50pm,7:07pm,Departure 35,7:30pm,7:45pm,7:50pm,8:07pm,Departure 36,8:00pm,8:15pm,8:20pm,8:37pm;Departure 1,8:00am,8:00am,8:15am,8:20am,8:37am,Departure 2,8:30am,8:30am,8:45am,8:50am,9:07am,Departure 3,9:00am,9:00am,9:15am,9:20am,9:37am,Departure 4,9:30am,9:30am,9:45am,9:50am,10:07am,Departure 5,10:00am,10:00am,10:15am,10:20am,10:37am,Departure 6,10:30am,10:30am,10:45am,10:50am,11:07am,Departure 7,11:00am,11:00am,11:15am,11:20am,11:37am,Departure 8,11:30am,11:30am,11:45am,11:50am,12:07pm,Departure 9,12:00pm,12:00pm,12:15pm,12:20pm,12:37pm,Departure 10,12:30pm,12:30pm,12:45pm,12:50pm,1:07pm,Departure 11,1:00pm,1:00pm,1:15pm,1:20pm,1:37pm,Departure 12,1:30pm,1:30pm,1:45pm,1:50pm,2:07pm,Departure 13,2:00pm,2:00pm,2:15pm,2:20pm,2:37pm,Departure 14,2:30pm,2:30pm,2:45pm,2:50pm,3:07pm,Departure 15,3:00pm,3:00pm,3:15pm,3:20pm,3:37pm,Departure 16,3:30pm,3:30pm,3:45pm,3:50pm,4:07pm,Departure 17,4:00pm,4:00pm,4:15pm,4:20pm,4:37pm,Departure 18,4:30pm,4:30pm,4:45pm,4:50pm,5:07pm,Departure 19,5:30pm,5:30pm,5:45pm,5:50pm,6:07pm,Departure 20,7:30pm,7:30pm,7:45pm,7:50pm,8:07pm,Departure 21,9:00pm,9:00pm,9:15pm,9:20pm,9:37pm,Departure 22,10:30pm,10:30pm,10:45pm,10:50pm,11:07pm;Departure 1,8:00am,8:00am,8:15am,8:20am,8:37am,Departure 2,8:30am,8:30am,8:45am,8:50am,9:07am,Departure 3,9:00am,9:00am,9:15am,9:20am,9:37am,Departure 4,9:30am,9:30am,9:45am,9:50am,10:07am,Departure 5,10:00am,10:00am,10:15am,10:20am,10:37am,Departure 6,10:30am,10:30am,10:45am,10:50am,11:07am,Departure 7,11:00am,11:00am,11:15am,11:20am,11:37am,Departure 8,11:30am,11:30am,11:45am,11:50am,12:07pm,Departure 9,12:00pm,12:00pm,12:15pm,12:20pm,12:37pm,Departure 10,12:30pm,12:30pm,12:45pm,12:50pm,1:07pm,Departure 11,1:00pm,1:00pm,1:15pm,1:20pm,1:37pm,Departure 12,1:30pm,1:30pm,1:45pm,1:50pm,2:07pm,Departure 13,2:00pm,2:00pm,2:15pm,2:20pm,2:37pm,Departure 14,2:30pm,2:30pm,2:45pm,2:50pm,3:07pm,Departure 15,3:00pm,3:00pm,3:15pm,3:20pm,3:37pm,Departure 16,3:30pm,3:30pm,3:45pm,3:50pm,4:07pm,Departure 17,4:00pm,4:00pm,4:15pm,4:20pm,4:37pm,Departure 18,4:30pm,4:30pm,4:45pm,4:50pm,5:07pm,Departure 19,5:30pm,5:30pm,5:45pm,5:50pm,6:07pm,Departure 20,7:30pm,7:30pm,7:45pm,7:50pm,8:07pm,Departure 21,9:00pm,9:00pm,9:15pm,9:20pm,9:37pm;Bus Hub Stop F;Green Is. (Outbound);Morris Rd, cnr Coach Rd;Mosgiel Terminus;Departure 1,7:12am,7:29am,7:35am,7:50am,Departure 2,7:42am,7:59am,8:05am,8:20am,Departure 3,7:57am,8:14am,8:20am,8:35am,Departure 4,8:12am,8:29am,8:35am,8:50am,Departure 5,8:27am,8:44am,8:50am,9:05am,Departure 6,8:42am,8:59am,9:05am,9:20am,Departure 7,8:57am,9:14am,9:20am,9:35am,Departure 8,9:12am,9:29am,9:35am,9:50am,Departure 9,9:42am,9:59am,10:05am,10:20am,Departure 10,10:12am,10:29am,10:35am,10:50am,Departure 11,10:42am,10:59am,11:05am,11:20am,Departure 12,11:12am,11:29am,11:35am,11:50am,Departure 13,11:42am,11:59am,12:05pm,12:20pm,Departure 14,12:12pm,12:29pm,12:35pm,12:50pm,Departure 15,12:42pm,12:59pm,1:05pm,1:20pm,Departure 16,1:12pm,1:29pm,1:35pm,1:50pm,Departure 17,1:42pm,1:59pm,2:05pm,2:20pm,Departure 18,2:12pm,2:29pm,2:35pm,2:50pm,Departure 19,2:42pm,2:59pm,3:05pm,3:20pm,Departure 20,3:12pm,3:29pm,3:35pm,3:50pm,Departure 21,3:42pm,3:59pm,4:05pm,4:20pm,Departure 22,3:57pm,4:14pm,4:20pm,4:35pm,Departure 23,4:12pm,4:29pm,4:35pm,4:50pm,Departure 24,4:27pm,4:44pm,4:50pm,5:05pm,Departure 25,4:42pm,4:59pm,5:05pm,5:20pm,Departure 26,4:57pm,5:14pm,5:20pm,5:35pm,Departure 27,5:12pm,5:29pm,5:35pm,5:50pm,Departure 28,5:27pm,5:44pm,5:50pm,6:05pm,Departure 29,5:42pm,5:59pm,6:05pm,6:20pm,Departure 30,6:12pm,6:29pm,6:35pm,6:50pm,Departure 31,6:42pm,6:59pm,7:05pm,7:20pm,Departure 32,7:12pm,7:29pm,7:35pm,7:50pm,Departure 33,8:42pm,8:59pm,9:05pm,9:20pm;Departure 1,7:12am,7:29am,7:35am,7:50am,Departure 2,7:42am,7:59am,8:05am,8:20am,Departure 3,7:57am,8:14am,8:20am,8:35am,Departure 4,8:12am,8:29am,8:35am,8:50am,Departure 5,8:27am,8:44am,8:50am,9:05am,Departure 6,8:42am,8:59am,9:05am,9:20am,Departure 7,8:57am,9:14am,9:20am,9:35am,Departure 8,9:12am,9:29am,9:35am,9:50am,Departure 9,9:42am,9:59am,10:05am,10:20am,Departure 10,10:12am,10:29am,10:35am,10:50am,Departure 11,10:42am,10:59am,11:05am,11:20am,Departure 12,11:12am,11:29am,11:35am,11:50am,Departure 13,11:42am,11:59am,12:05pm,12:20pm,Departure 14,12:12pm,12:29pm,12:35pm,12:50pm,Departure 15,12:42pm,12:59pm,1:05pm,1:20pm,Departure 16,1:12pm,1:29pm,1:35pm,1:50pm,Departure 17,1:42pm,1:59pm,2:05pm,2:20pm,Departure 18,2:12pm,2:29pm,2:35pm,2:50pm,Departure 19,2:42pm,2:59pm,3:05pm,3:20pm,Departure 20,3:12pm,3:29pm,3:35pm,3:50pm,Departure 21,3:42pm,3:59pm,4:05pm,4:20pm,Departure 22,3:57pm,4:14pm,4:20pm,4:35pm,Departure 23,4:12pm,4:29pm,4:35pm,4:50pm,Departure 24,4:27pm,4:44pm,4:50pm,5:05pm,Departure 25,4:42pm,4:59pm,5:05pm,5:20pm,Departure 26,4:57pm,5:14pm,5:20pm,5:35pm,Departure 27,5:12pm,5:29pm,5:35pm,5:50pm,Departure 28,5:27pm,5:44pm,5:50pm,6:05pm,Departure 29,5:42pm,5:59pm,6:05pm,6:20pm,Departure 30,6:12pm,6:29pm,6:35pm,6:50pm,Departure 31,6:42pm,6:59pm,7:05pm,7:20pm,Departure 32,7:12pm,7:29pm,7:35pm,7:50pm,Departure 33,8:42pm,8:59pm,9:05pm,9:20pm,Departure 34,11:42pm,11:59pm,12:05am,12:20am;Departure 1,8:42am,8:59am,9:05am,9:20am,Departure 2,9:12am,9:29am,9:35am,9:50am,Departure 3,9:42am,9:59am,10:05am,10:20am,Departure 4,10:12am,10:29am,10:35am,10:50am,Departure 5,10:42am,10:59am,11:05am,11:20am,Departure 6,11:12am,11:29am,11:35am,11:50am,Departure 7,11:42am,11:59am,12:05pm,12:20pm,Departure 8,12:12pm,12:29pm,12:35pm,12:50pm,Departure 9,12:42pm,12:59pm,1:05pm,1:20pm,Departure 10,1:12pm,1:29pm,1:35pm,1:50pm,Departure 11,1:42pm,1:59pm,2:05pm,2:20pm,Departure 12,2:12pm,2:29pm,2:35pm,2:50pm,Departure 13,2:42pm,2:59pm,3:05pm,3:20pm,Departure 14,3:12pm,3:29pm,3:35pm,3:50pm,Departure 15,3:42pm,3:59pm,4:05pm,4:20pm,Departure 16,4:42pm,4:59pm,5:05pm,5:20pm,Departure 17,6:12pm,6:29pm,6:35pm,6:50pm,Departure 18,8:12pm,8:29pm,8:35pm,8:50pm,Departure 19,9:42pm,9:59pm,10:05pm,10:20pm,Departure 20,11:42pm,11:59pm,12:05am,12:20am;Departure 1,8:42am,8:59am,9:05am,9:20am,Departure 2,9:12am,9:29am,9:35am,9:50am,Departure 3,9:42am,9:59am,10:05am,10:20am,Departure 4,10:12am,10:29am,10:35am,10:50am,Departure 5,10:42am,10:59am,11:05am,11:20am,Departure 6,11:12am,11:29am,11:35am,11:50am,Departure 7,11:42am,11:59am,12:05pm,12:20pm,Departure 8,12:12pm,12:29pm,12:35pm,12:50pm,Departure 9,12:42pm,12:59pm,1:05pm,1:20pm,Departure 10,1:12pm,1:29pm,1:35pm,1:50pm,Departure 11,1:42pm,1:59pm,2:05pm,2:20pm,Departure 12,2:12pm,2:29pm,2:35pm,2:50pm,Departure 13,2:42pm,2:59pm,3:05pm,3:20pm,Departure 14,3:12pm,3:29pm,3:35pm,3:50pm,Departure 15,3:42pm,3:59pm,4:05pm,4:20pm,Departure 16,4:42pm,4:59pm,5:05pm,5:20pm,Departure 17,6:12pm,6:29pm,6:35pm,6:50pm,Departure 18,8:12pm,8:29pm,8:35pm,8:50pm,Departure 19,9:42pm,9:59pm,10:05pm,10:20pm</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -21367,6 +21398,78 @@
       </c>
       <c r="B29" t="s">
         <v>992</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>995</v>
+      </c>
+      <c r="B30" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>721</v>
+      </c>
+      <c r="B31" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>722</v>
+      </c>
+      <c r="B32" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>723</v>
+      </c>
+      <c r="B33" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>998</v>
+      </c>
+      <c r="B34" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>726</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>727</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>722</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>723</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>